<commit_message>
Update GSW playoffs json & spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3367,6 +3367,2848 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>24:18</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>4</v>
+      </c>
+      <c r="J32" t="n">
+        <v>7</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="L32" t="n">
+        <v>3</v>
+      </c>
+      <c r="M32" t="n">
+        <v>6</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>2</v>
+      </c>
+      <c r="T32" t="n">
+        <v>2</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1</v>
+      </c>
+      <c r="V32" t="n">
+        <v>1</v>
+      </c>
+      <c r="W32" t="n">
+        <v>1</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>7:52</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2</v>
+      </c>
+      <c r="T33" t="n">
+        <v>2</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>30:35</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>2</v>
+      </c>
+      <c r="J34" t="n">
+        <v>6</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L34" t="n">
+        <v>2</v>
+      </c>
+      <c r="M34" t="n">
+        <v>6</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O34" t="n">
+        <v>2</v>
+      </c>
+      <c r="P34" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1</v>
+      </c>
+      <c r="S34" t="n">
+        <v>4</v>
+      </c>
+      <c r="T34" t="n">
+        <v>5</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1</v>
+      </c>
+      <c r="V34" t="n">
+        <v>3</v>
+      </c>
+      <c r="W34" t="n">
+        <v>1</v>
+      </c>
+      <c r="X34" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>14:08</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>5</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>2</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>37:20</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" t="n">
+        <v>15</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L36" t="n">
+        <v>4</v>
+      </c>
+      <c r="M36" t="n">
+        <v>9</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="O36" t="n">
+        <v>4</v>
+      </c>
+      <c r="P36" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="n">
+        <v>5</v>
+      </c>
+      <c r="T36" t="n">
+        <v>5</v>
+      </c>
+      <c r="U36" t="n">
+        <v>9</v>
+      </c>
+      <c r="V36" t="n">
+        <v>1</v>
+      </c>
+      <c r="W36" t="n">
+        <v>1</v>
+      </c>
+      <c r="X36" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>3</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>1</v>
+      </c>
+      <c r="U37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V37" t="n">
+        <v>1</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0</v>
+      </c>
+      <c r="X37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>24:39</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>4</v>
+      </c>
+      <c r="J38" t="n">
+        <v>9</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="L38" t="n">
+        <v>4</v>
+      </c>
+      <c r="M38" t="n">
+        <v>8</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>2</v>
+      </c>
+      <c r="T38" t="n">
+        <v>2</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1</v>
+      </c>
+      <c r="V38" t="n">
+        <v>1</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="n">
+        <v>3</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1</v>
+      </c>
+      <c r="S39" t="n">
+        <v>3</v>
+      </c>
+      <c r="T39" t="n">
+        <v>4</v>
+      </c>
+      <c r="U39" t="n">
+        <v>1</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>2</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>1</v>
+      </c>
+      <c r="P40" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R40" t="n">
+        <v>2</v>
+      </c>
+      <c r="S40" t="n">
+        <v>2</v>
+      </c>
+      <c r="T40" t="n">
+        <v>4</v>
+      </c>
+      <c r="U40" t="n">
+        <v>3</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="n">
+        <v>0</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" t="n">
+        <v>3</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>1</v>
+      </c>
+      <c r="P41" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1</v>
+      </c>
+      <c r="U41" t="n">
+        <v>1</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="n">
+        <v>0</v>
+      </c>
+      <c r="X41" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>26:04</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>4</v>
+      </c>
+      <c r="J42" t="n">
+        <v>12</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L42" t="n">
+        <v>2</v>
+      </c>
+      <c r="M42" t="n">
+        <v>5</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1</v>
+      </c>
+      <c r="P42" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R42" t="n">
+        <v>1</v>
+      </c>
+      <c r="S42" t="n">
+        <v>2</v>
+      </c>
+      <c r="T42" t="n">
+        <v>3</v>
+      </c>
+      <c r="U42" t="n">
+        <v>2</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="n">
+        <v>1</v>
+      </c>
+      <c r="X42" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>5</v>
+      </c>
+      <c r="J43" t="n">
+        <v>7</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="L43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M43" t="n">
+        <v>1</v>
+      </c>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1</v>
+      </c>
+      <c r="U43" t="n">
+        <v>1</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" t="n">
+        <v>0</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>3:40</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="n">
+        <v>1</v>
+      </c>
+      <c r="S44" t="n">
+        <v>1</v>
+      </c>
+      <c r="T44" t="n">
+        <v>2</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" t="n">
+        <v>0</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>3:40</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" t="n">
+        <v>2</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>3:40</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="n">
+        <v>3</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>1</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T46" t="n">
+        <v>1</v>
+      </c>
+      <c r="U46" t="n">
+        <v>1</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" t="n">
+        <v>0</v>
+      </c>
+      <c r="X46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1628415</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Dillon Brooks</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>24:48</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>6</v>
+      </c>
+      <c r="J47" t="n">
+        <v>12</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L47" t="n">
+        <v>2</v>
+      </c>
+      <c r="M47" t="n">
+        <v>5</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O47" t="n">
+        <v>2</v>
+      </c>
+      <c r="P47" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>1</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>3</v>
+      </c>
+      <c r="T47" t="n">
+        <v>3</v>
+      </c>
+      <c r="U47" t="n">
+        <v>1</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" t="n">
+        <v>1</v>
+      </c>
+      <c r="X47" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1641708</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Amen Thompson</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>22:42</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>4</v>
+      </c>
+      <c r="J48" t="n">
+        <v>7</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="n">
+        <v>1</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>3</v>
+      </c>
+      <c r="P48" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1</v>
+      </c>
+      <c r="T48" t="n">
+        <v>1</v>
+      </c>
+      <c r="U48" t="n">
+        <v>3</v>
+      </c>
+      <c r="V48" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="n">
+        <v>0</v>
+      </c>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1630578</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Alperen Sengun</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>36:47</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>6</v>
+      </c>
+      <c r="J49" t="n">
+        <v>15</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L49" t="n">
+        <v>1</v>
+      </c>
+      <c r="M49" t="n">
+        <v>2</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O49" t="n">
+        <v>4</v>
+      </c>
+      <c r="P49" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R49" t="n">
+        <v>6</v>
+      </c>
+      <c r="S49" t="n">
+        <v>10</v>
+      </c>
+      <c r="T49" t="n">
+        <v>16</v>
+      </c>
+      <c r="U49" t="n">
+        <v>7</v>
+      </c>
+      <c r="V49" t="n">
+        <v>2</v>
+      </c>
+      <c r="W49" t="n">
+        <v>0</v>
+      </c>
+      <c r="X49" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1630224</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Jalen Green</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>35:20</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>13</v>
+      </c>
+      <c r="J50" t="n">
+        <v>25</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="L50" t="n">
+        <v>8</v>
+      </c>
+      <c r="M50" t="n">
+        <v>18</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="O50" t="n">
+        <v>4</v>
+      </c>
+      <c r="P50" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>4</v>
+      </c>
+      <c r="T50" t="n">
+        <v>4</v>
+      </c>
+      <c r="U50" t="n">
+        <v>6</v>
+      </c>
+      <c r="V50" t="n">
+        <v>3</v>
+      </c>
+      <c r="W50" t="n">
+        <v>0</v>
+      </c>
+      <c r="X50" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>38</v>
+      </c>
+      <c r="AA50" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1627832</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Fred VanVleet</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>42:14</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>2</v>
+      </c>
+      <c r="J51" t="n">
+        <v>8</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L51" t="n">
+        <v>1</v>
+      </c>
+      <c r="M51" t="n">
+        <v>7</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="O51" t="n">
+        <v>2</v>
+      </c>
+      <c r="P51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>1</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="n">
+        <v>6</v>
+      </c>
+      <c r="T51" t="n">
+        <v>6</v>
+      </c>
+      <c r="U51" t="n">
+        <v>2</v>
+      </c>
+      <c r="V51" t="n">
+        <v>3</v>
+      </c>
+      <c r="W51" t="n">
+        <v>1</v>
+      </c>
+      <c r="X51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1631106</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Tari Eason</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>24:19</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>6</v>
+      </c>
+      <c r="J52" t="n">
+        <v>9</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="L52" t="n">
+        <v>2</v>
+      </c>
+      <c r="M52" t="n">
+        <v>2</v>
+      </c>
+      <c r="N52" t="n">
+        <v>1</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>3</v>
+      </c>
+      <c r="S52" t="n">
+        <v>3</v>
+      </c>
+      <c r="T52" t="n">
+        <v>6</v>
+      </c>
+      <c r="U52" t="n">
+        <v>1</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0</v>
+      </c>
+      <c r="X52" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1631095</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Jabari Smith Jr.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>23:51</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>2</v>
+      </c>
+      <c r="J53" t="n">
+        <v>4</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L53" t="n">
+        <v>1</v>
+      </c>
+      <c r="M53" t="n">
+        <v>3</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="n">
+        <v>5</v>
+      </c>
+      <c r="T53" t="n">
+        <v>5</v>
+      </c>
+      <c r="U53" t="n">
+        <v>0</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" t="n">
+        <v>1</v>
+      </c>
+      <c r="X53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>203500</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Steven Adams</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>1</v>
+      </c>
+      <c r="P54" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R54" t="n">
+        <v>1</v>
+      </c>
+      <c r="S54" t="n">
+        <v>2</v>
+      </c>
+      <c r="T54" t="n">
+        <v>3</v>
+      </c>
+      <c r="U54" t="n">
+        <v>0</v>
+      </c>
+      <c r="V54" t="n">
+        <v>1</v>
+      </c>
+      <c r="W54" t="n">
+        <v>1</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1628988</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Aaron Holiday</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>5:12</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>2</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>1</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="n">
+        <v>1</v>
+      </c>
+      <c r="T55" t="n">
+        <v>1</v>
+      </c>
+      <c r="U55" t="n">
+        <v>1</v>
+      </c>
+      <c r="V55" t="n">
+        <v>0</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>201145</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Jeff Green</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>2</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0</v>
+      </c>
+      <c r="R56" t="n">
+        <v>1</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0</v>
+      </c>
+      <c r="T56" t="n">
+        <v>1</v>
+      </c>
+      <c r="U56" t="n">
+        <v>0</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0</v>
+      </c>
+      <c r="X56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1641715</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Cam Whitmore</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" t="n">
+        <v>1</v>
+      </c>
+      <c r="T57" t="n">
+        <v>1</v>
+      </c>
+      <c r="U57" t="n">
+        <v>0</v>
+      </c>
+      <c r="V57" t="n">
+        <v>0</v>
+      </c>
+      <c r="W57" t="n">
+        <v>0</v>
+      </c>
+      <c r="X57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1631466</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Nate Williams</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0</v>
+      </c>
+      <c r="U58" t="n">
+        <v>0</v>
+      </c>
+      <c r="V58" t="n">
+        <v>0</v>
+      </c>
+      <c r="W58" t="n">
+        <v>0</v>
+      </c>
+      <c r="X58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1642263</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Reed Sheppard</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>1</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0</v>
+      </c>
+      <c r="T59" t="n">
+        <v>0</v>
+      </c>
+      <c r="U59" t="n">
+        <v>0</v>
+      </c>
+      <c r="V59" t="n">
+        <v>0</v>
+      </c>
+      <c r="W59" t="n">
+        <v>0</v>
+      </c>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1629111</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Jock Landale</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="n">
+        <v>0</v>
+      </c>
+      <c r="T60" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0</v>
+      </c>
+      <c r="W60" t="n">
+        <v>0</v>
+      </c>
+      <c r="X60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1630256</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Jae'Sean Tate</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="n">
+        <v>0</v>
+      </c>
+      <c r="T61" t="n">
+        <v>0</v>
+      </c>
+      <c r="U61" t="n">
+        <v>0</v>
+      </c>
+      <c r="V61" t="n">
+        <v>0</v>
+      </c>
+      <c r="W61" t="n">
+        <v>0</v>
+      </c>
+      <c r="X61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add GSW vs HOU GM5 stats & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA121"/>
+  <dimension ref="A1:AA151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11813,6 +11813,2848 @@
         <v>0</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
+        <v>2</v>
+      </c>
+      <c r="J122" t="n">
+        <v>6</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="n">
+        <v>2</v>
+      </c>
+      <c r="N122" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="n">
+        <v>0</v>
+      </c>
+      <c r="P122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>0</v>
+      </c>
+      <c r="R122" t="n">
+        <v>2</v>
+      </c>
+      <c r="S122" t="n">
+        <v>0</v>
+      </c>
+      <c r="T122" t="n">
+        <v>2</v>
+      </c>
+      <c r="U122" t="n">
+        <v>1</v>
+      </c>
+      <c r="V122" t="n">
+        <v>1</v>
+      </c>
+      <c r="W122" t="n">
+        <v>1</v>
+      </c>
+      <c r="X122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y122" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z122" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA122" t="n">
+        <v>-22</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>25:21</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
+        <v>2</v>
+      </c>
+      <c r="J123" t="n">
+        <v>10</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L123" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="n">
+        <v>3</v>
+      </c>
+      <c r="N123" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="n">
+        <v>4</v>
+      </c>
+      <c r="P123" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R123" t="n">
+        <v>4</v>
+      </c>
+      <c r="S123" t="n">
+        <v>1</v>
+      </c>
+      <c r="T123" t="n">
+        <v>5</v>
+      </c>
+      <c r="U123" t="n">
+        <v>2</v>
+      </c>
+      <c r="V123" t="n">
+        <v>2</v>
+      </c>
+      <c r="W123" t="n">
+        <v>0</v>
+      </c>
+      <c r="X123" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y123" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z123" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA123" t="n">
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="I124" t="n">
+        <v>3</v>
+      </c>
+      <c r="J124" t="n">
+        <v>4</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L124" t="n">
+        <v>1</v>
+      </c>
+      <c r="M124" t="n">
+        <v>2</v>
+      </c>
+      <c r="N124" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O124" t="n">
+        <v>0</v>
+      </c>
+      <c r="P124" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>0</v>
+      </c>
+      <c r="R124" t="n">
+        <v>0</v>
+      </c>
+      <c r="S124" t="n">
+        <v>1</v>
+      </c>
+      <c r="T124" t="n">
+        <v>1</v>
+      </c>
+      <c r="U124" t="n">
+        <v>1</v>
+      </c>
+      <c r="V124" t="n">
+        <v>2</v>
+      </c>
+      <c r="W124" t="n">
+        <v>0</v>
+      </c>
+      <c r="X124" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y124" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z124" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA124" t="n">
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>20:54</t>
+        </is>
+      </c>
+      <c r="I125" t="n">
+        <v>3</v>
+      </c>
+      <c r="J125" t="n">
+        <v>7</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="L125" t="n">
+        <v>2</v>
+      </c>
+      <c r="M125" t="n">
+        <v>4</v>
+      </c>
+      <c r="N125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O125" t="n">
+        <v>0</v>
+      </c>
+      <c r="P125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>0</v>
+      </c>
+      <c r="R125" t="n">
+        <v>0</v>
+      </c>
+      <c r="S125" t="n">
+        <v>2</v>
+      </c>
+      <c r="T125" t="n">
+        <v>2</v>
+      </c>
+      <c r="U125" t="n">
+        <v>4</v>
+      </c>
+      <c r="V125" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="n">
+        <v>0</v>
+      </c>
+      <c r="X125" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y125" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z125" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA125" t="n">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>23:26</t>
+        </is>
+      </c>
+      <c r="I126" t="n">
+        <v>4</v>
+      </c>
+      <c r="J126" t="n">
+        <v>12</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L126" t="n">
+        <v>3</v>
+      </c>
+      <c r="M126" t="n">
+        <v>9</v>
+      </c>
+      <c r="N126" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O126" t="n">
+        <v>2</v>
+      </c>
+      <c r="P126" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="R126" t="n">
+        <v>1</v>
+      </c>
+      <c r="S126" t="n">
+        <v>2</v>
+      </c>
+      <c r="T126" t="n">
+        <v>3</v>
+      </c>
+      <c r="U126" t="n">
+        <v>7</v>
+      </c>
+      <c r="V126" t="n">
+        <v>0</v>
+      </c>
+      <c r="W126" t="n">
+        <v>0</v>
+      </c>
+      <c r="X126" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y126" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z126" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA126" t="n">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="I127" t="n">
+        <v>2</v>
+      </c>
+      <c r="J127" t="n">
+        <v>4</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L127" t="n">
+        <v>1</v>
+      </c>
+      <c r="M127" t="n">
+        <v>2</v>
+      </c>
+      <c r="N127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O127" t="n">
+        <v>0</v>
+      </c>
+      <c r="P127" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="n">
+        <v>0</v>
+      </c>
+      <c r="R127" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" t="n">
+        <v>2</v>
+      </c>
+      <c r="T127" t="n">
+        <v>2</v>
+      </c>
+      <c r="U127" t="n">
+        <v>0</v>
+      </c>
+      <c r="V127" t="n">
+        <v>0</v>
+      </c>
+      <c r="W127" t="n">
+        <v>2</v>
+      </c>
+      <c r="X127" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y127" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z127" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA127" t="n">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="I128" t="n">
+        <v>3</v>
+      </c>
+      <c r="J128" t="n">
+        <v>6</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L128" t="n">
+        <v>2</v>
+      </c>
+      <c r="M128" t="n">
+        <v>5</v>
+      </c>
+      <c r="N128" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="n">
+        <v>0</v>
+      </c>
+      <c r="R128" t="n">
+        <v>0</v>
+      </c>
+      <c r="S128" t="n">
+        <v>1</v>
+      </c>
+      <c r="T128" t="n">
+        <v>1</v>
+      </c>
+      <c r="U128" t="n">
+        <v>2</v>
+      </c>
+      <c r="V128" t="n">
+        <v>0</v>
+      </c>
+      <c r="W128" t="n">
+        <v>0</v>
+      </c>
+      <c r="X128" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y128" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z128" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA128" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="I129" t="n">
+        <v>2</v>
+      </c>
+      <c r="J129" t="n">
+        <v>4</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L129" t="n">
+        <v>2</v>
+      </c>
+      <c r="M129" t="n">
+        <v>4</v>
+      </c>
+      <c r="N129" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O129" t="n">
+        <v>1</v>
+      </c>
+      <c r="P129" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q129" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R129" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="n">
+        <v>2</v>
+      </c>
+      <c r="T129" t="n">
+        <v>2</v>
+      </c>
+      <c r="U129" t="n">
+        <v>2</v>
+      </c>
+      <c r="V129" t="n">
+        <v>0</v>
+      </c>
+      <c r="W129" t="n">
+        <v>0</v>
+      </c>
+      <c r="X129" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y129" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z129" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA129" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>25:56</t>
+        </is>
+      </c>
+      <c r="I130" t="n">
+        <v>9</v>
+      </c>
+      <c r="J130" t="n">
+        <v>18</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L130" t="n">
+        <v>3</v>
+      </c>
+      <c r="M130" t="n">
+        <v>7</v>
+      </c>
+      <c r="N130" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="O130" t="n">
+        <v>4</v>
+      </c>
+      <c r="P130" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>1</v>
+      </c>
+      <c r="R130" t="n">
+        <v>5</v>
+      </c>
+      <c r="S130" t="n">
+        <v>4</v>
+      </c>
+      <c r="T130" t="n">
+        <v>9</v>
+      </c>
+      <c r="U130" t="n">
+        <v>2</v>
+      </c>
+      <c r="V130" t="n">
+        <v>2</v>
+      </c>
+      <c r="W130" t="n">
+        <v>1</v>
+      </c>
+      <c r="X130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y130" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z130" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA130" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
+        <v>1</v>
+      </c>
+      <c r="J131" t="n">
+        <v>3</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
+      <c r="R131" t="n">
+        <v>2</v>
+      </c>
+      <c r="S131" t="n">
+        <v>1</v>
+      </c>
+      <c r="T131" t="n">
+        <v>3</v>
+      </c>
+      <c r="U131" t="n">
+        <v>0</v>
+      </c>
+      <c r="V131" t="n">
+        <v>0</v>
+      </c>
+      <c r="W131" t="n">
+        <v>0</v>
+      </c>
+      <c r="X131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y131" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z131" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="I132" t="n">
+        <v>5</v>
+      </c>
+      <c r="J132" t="n">
+        <v>7</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="n">
+        <v>1</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" t="n">
+        <v>1</v>
+      </c>
+      <c r="P132" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q132" t="n">
+        <v>1</v>
+      </c>
+      <c r="R132" t="n">
+        <v>2</v>
+      </c>
+      <c r="S132" t="n">
+        <v>2</v>
+      </c>
+      <c r="T132" t="n">
+        <v>4</v>
+      </c>
+      <c r="U132" t="n">
+        <v>2</v>
+      </c>
+      <c r="V132" t="n">
+        <v>1</v>
+      </c>
+      <c r="W132" t="n">
+        <v>0</v>
+      </c>
+      <c r="X132" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y132" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z132" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA132" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="I133" t="n">
+        <v>5</v>
+      </c>
+      <c r="J133" t="n">
+        <v>13</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="L133" t="n">
+        <v>1</v>
+      </c>
+      <c r="M133" t="n">
+        <v>4</v>
+      </c>
+      <c r="N133" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O133" t="n">
+        <v>3</v>
+      </c>
+      <c r="P133" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>1</v>
+      </c>
+      <c r="R133" t="n">
+        <v>2</v>
+      </c>
+      <c r="S133" t="n">
+        <v>2</v>
+      </c>
+      <c r="T133" t="n">
+        <v>4</v>
+      </c>
+      <c r="U133" t="n">
+        <v>2</v>
+      </c>
+      <c r="V133" t="n">
+        <v>0</v>
+      </c>
+      <c r="W133" t="n">
+        <v>1</v>
+      </c>
+      <c r="X133" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y133" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z133" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA133" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="I134" t="n">
+        <v>2</v>
+      </c>
+      <c r="J134" t="n">
+        <v>2</v>
+      </c>
+      <c r="K134" t="n">
+        <v>1</v>
+      </c>
+      <c r="L134" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" t="n">
+        <v>0</v>
+      </c>
+      <c r="N134" t="n">
+        <v>0</v>
+      </c>
+      <c r="O134" t="n">
+        <v>0</v>
+      </c>
+      <c r="P134" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q134" t="n">
+        <v>0</v>
+      </c>
+      <c r="R134" t="n">
+        <v>2</v>
+      </c>
+      <c r="S134" t="n">
+        <v>2</v>
+      </c>
+      <c r="T134" t="n">
+        <v>4</v>
+      </c>
+      <c r="U134" t="n">
+        <v>0</v>
+      </c>
+      <c r="V134" t="n">
+        <v>1</v>
+      </c>
+      <c r="W134" t="n">
+        <v>0</v>
+      </c>
+      <c r="X134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y134" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z134" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA134" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" t="n">
+        <v>7</v>
+      </c>
+      <c r="K135" t="n">
+        <v>0</v>
+      </c>
+      <c r="L135" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" t="n">
+        <v>1</v>
+      </c>
+      <c r="N135" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" t="n">
+        <v>0</v>
+      </c>
+      <c r="P135" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="n">
+        <v>0</v>
+      </c>
+      <c r="R135" t="n">
+        <v>5</v>
+      </c>
+      <c r="S135" t="n">
+        <v>2</v>
+      </c>
+      <c r="T135" t="n">
+        <v>7</v>
+      </c>
+      <c r="U135" t="n">
+        <v>0</v>
+      </c>
+      <c r="V135" t="n">
+        <v>1</v>
+      </c>
+      <c r="W135" t="n">
+        <v>0</v>
+      </c>
+      <c r="X135" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y135" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z135" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA135" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0</v>
+      </c>
+      <c r="N136" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" t="n">
+        <v>0</v>
+      </c>
+      <c r="P136" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="n">
+        <v>0</v>
+      </c>
+      <c r="R136" t="n">
+        <v>0</v>
+      </c>
+      <c r="S136" t="n">
+        <v>0</v>
+      </c>
+      <c r="T136" t="n">
+        <v>0</v>
+      </c>
+      <c r="U136" t="n">
+        <v>0</v>
+      </c>
+      <c r="V136" t="n">
+        <v>0</v>
+      </c>
+      <c r="W136" t="n">
+        <v>0</v>
+      </c>
+      <c r="X136" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y136" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1628415</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Dillon Brooks</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>28:59</t>
+        </is>
+      </c>
+      <c r="I137" t="n">
+        <v>7</v>
+      </c>
+      <c r="J137" t="n">
+        <v>13</v>
+      </c>
+      <c r="K137" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="L137" t="n">
+        <v>2</v>
+      </c>
+      <c r="M137" t="n">
+        <v>7</v>
+      </c>
+      <c r="N137" t="n">
+        <v>0.286</v>
+      </c>
+      <c r="O137" t="n">
+        <v>8</v>
+      </c>
+      <c r="P137" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q137" t="n">
+        <v>1</v>
+      </c>
+      <c r="R137" t="n">
+        <v>0</v>
+      </c>
+      <c r="S137" t="n">
+        <v>1</v>
+      </c>
+      <c r="T137" t="n">
+        <v>1</v>
+      </c>
+      <c r="U137" t="n">
+        <v>2</v>
+      </c>
+      <c r="V137" t="n">
+        <v>0</v>
+      </c>
+      <c r="W137" t="n">
+        <v>0</v>
+      </c>
+      <c r="X137" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y137" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z137" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA137" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1641708</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Amen Thompson</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>34:41</t>
+        </is>
+      </c>
+      <c r="I138" t="n">
+        <v>8</v>
+      </c>
+      <c r="J138" t="n">
+        <v>12</v>
+      </c>
+      <c r="K138" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="L138" t="n">
+        <v>1</v>
+      </c>
+      <c r="M138" t="n">
+        <v>1</v>
+      </c>
+      <c r="N138" t="n">
+        <v>1</v>
+      </c>
+      <c r="O138" t="n">
+        <v>8</v>
+      </c>
+      <c r="P138" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="R138" t="n">
+        <v>4</v>
+      </c>
+      <c r="S138" t="n">
+        <v>2</v>
+      </c>
+      <c r="T138" t="n">
+        <v>6</v>
+      </c>
+      <c r="U138" t="n">
+        <v>3</v>
+      </c>
+      <c r="V138" t="n">
+        <v>5</v>
+      </c>
+      <c r="W138" t="n">
+        <v>3</v>
+      </c>
+      <c r="X138" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y138" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z138" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA138" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>1630578</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Alperen Sengun</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>30:50</t>
+        </is>
+      </c>
+      <c r="I139" t="n">
+        <v>6</v>
+      </c>
+      <c r="J139" t="n">
+        <v>9</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="n">
+        <v>3</v>
+      </c>
+      <c r="P139" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R139" t="n">
+        <v>1</v>
+      </c>
+      <c r="S139" t="n">
+        <v>8</v>
+      </c>
+      <c r="T139" t="n">
+        <v>9</v>
+      </c>
+      <c r="U139" t="n">
+        <v>9</v>
+      </c>
+      <c r="V139" t="n">
+        <v>2</v>
+      </c>
+      <c r="W139" t="n">
+        <v>2</v>
+      </c>
+      <c r="X139" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y139" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z139" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA139" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1630224</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Jalen Green</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>27:50</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
+        <v>3</v>
+      </c>
+      <c r="J140" t="n">
+        <v>8</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="L140" t="n">
+        <v>2</v>
+      </c>
+      <c r="M140" t="n">
+        <v>4</v>
+      </c>
+      <c r="N140" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O140" t="n">
+        <v>3</v>
+      </c>
+      <c r="P140" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="R140" t="n">
+        <v>0</v>
+      </c>
+      <c r="S140" t="n">
+        <v>8</v>
+      </c>
+      <c r="T140" t="n">
+        <v>8</v>
+      </c>
+      <c r="U140" t="n">
+        <v>2</v>
+      </c>
+      <c r="V140" t="n">
+        <v>0</v>
+      </c>
+      <c r="W140" t="n">
+        <v>0</v>
+      </c>
+      <c r="X140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z140" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA140" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>1627832</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Fred VanVleet</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>33:07</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
+        <v>8</v>
+      </c>
+      <c r="J141" t="n">
+        <v>13</v>
+      </c>
+      <c r="K141" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="L141" t="n">
+        <v>4</v>
+      </c>
+      <c r="M141" t="n">
+        <v>6</v>
+      </c>
+      <c r="N141" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O141" t="n">
+        <v>6</v>
+      </c>
+      <c r="P141" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q141" t="n">
+        <v>1</v>
+      </c>
+      <c r="R141" t="n">
+        <v>0</v>
+      </c>
+      <c r="S141" t="n">
+        <v>1</v>
+      </c>
+      <c r="T141" t="n">
+        <v>1</v>
+      </c>
+      <c r="U141" t="n">
+        <v>2</v>
+      </c>
+      <c r="V141" t="n">
+        <v>0</v>
+      </c>
+      <c r="W141" t="n">
+        <v>1</v>
+      </c>
+      <c r="X141" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y141" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z141" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA141" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>203500</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Steven Adams</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>17:09</t>
+        </is>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>2</v>
+      </c>
+      <c r="K142" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" t="n">
+        <v>0</v>
+      </c>
+      <c r="N142" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" t="n">
+        <v>0</v>
+      </c>
+      <c r="P142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="n">
+        <v>0</v>
+      </c>
+      <c r="R142" t="n">
+        <v>3</v>
+      </c>
+      <c r="S142" t="n">
+        <v>3</v>
+      </c>
+      <c r="T142" t="n">
+        <v>6</v>
+      </c>
+      <c r="U142" t="n">
+        <v>1</v>
+      </c>
+      <c r="V142" t="n">
+        <v>0</v>
+      </c>
+      <c r="W142" t="n">
+        <v>0</v>
+      </c>
+      <c r="X142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y142" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA142" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>1631106</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Tari Eason</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="I143" t="n">
+        <v>4</v>
+      </c>
+      <c r="J143" t="n">
+        <v>5</v>
+      </c>
+      <c r="K143" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L143" t="n">
+        <v>1</v>
+      </c>
+      <c r="M143" t="n">
+        <v>2</v>
+      </c>
+      <c r="N143" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O143" t="n">
+        <v>0</v>
+      </c>
+      <c r="P143" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="n">
+        <v>0</v>
+      </c>
+      <c r="R143" t="n">
+        <v>0</v>
+      </c>
+      <c r="S143" t="n">
+        <v>5</v>
+      </c>
+      <c r="T143" t="n">
+        <v>5</v>
+      </c>
+      <c r="U143" t="n">
+        <v>1</v>
+      </c>
+      <c r="V143" t="n">
+        <v>0</v>
+      </c>
+      <c r="W143" t="n">
+        <v>0</v>
+      </c>
+      <c r="X143" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y143" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z143" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA143" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>1628988</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Aaron Holiday</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="I144" t="n">
+        <v>3</v>
+      </c>
+      <c r="J144" t="n">
+        <v>6</v>
+      </c>
+      <c r="K144" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L144" t="n">
+        <v>1</v>
+      </c>
+      <c r="M144" t="n">
+        <v>3</v>
+      </c>
+      <c r="N144" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O144" t="n">
+        <v>2</v>
+      </c>
+      <c r="P144" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q144" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R144" t="n">
+        <v>0</v>
+      </c>
+      <c r="S144" t="n">
+        <v>0</v>
+      </c>
+      <c r="T144" t="n">
+        <v>0</v>
+      </c>
+      <c r="U144" t="n">
+        <v>2</v>
+      </c>
+      <c r="V144" t="n">
+        <v>0</v>
+      </c>
+      <c r="W144" t="n">
+        <v>0</v>
+      </c>
+      <c r="X144" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y144" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z144" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA144" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1631095</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Jabari Smith Jr.</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>15:09</t>
+        </is>
+      </c>
+      <c r="I145" t="n">
+        <v>2</v>
+      </c>
+      <c r="J145" t="n">
+        <v>6</v>
+      </c>
+      <c r="K145" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L145" t="n">
+        <v>1</v>
+      </c>
+      <c r="M145" t="n">
+        <v>5</v>
+      </c>
+      <c r="N145" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O145" t="n">
+        <v>2</v>
+      </c>
+      <c r="P145" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q145" t="n">
+        <v>1</v>
+      </c>
+      <c r="R145" t="n">
+        <v>0</v>
+      </c>
+      <c r="S145" t="n">
+        <v>2</v>
+      </c>
+      <c r="T145" t="n">
+        <v>2</v>
+      </c>
+      <c r="U145" t="n">
+        <v>0</v>
+      </c>
+      <c r="V145" t="n">
+        <v>0</v>
+      </c>
+      <c r="W145" t="n">
+        <v>0</v>
+      </c>
+      <c r="X145" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y145" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z145" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA145" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>1642263</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Reed Sheppard</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>6:34</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>0</v>
+      </c>
+      <c r="R146" t="n">
+        <v>0</v>
+      </c>
+      <c r="S146" t="n">
+        <v>1</v>
+      </c>
+      <c r="T146" t="n">
+        <v>1</v>
+      </c>
+      <c r="U146" t="n">
+        <v>1</v>
+      </c>
+      <c r="V146" t="n">
+        <v>2</v>
+      </c>
+      <c r="W146" t="n">
+        <v>1</v>
+      </c>
+      <c r="X146" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y146" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA146" t="n">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>1629111</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Jock Landale</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>4:51</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
+        <v>1</v>
+      </c>
+      <c r="J147" t="n">
+        <v>2</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L147" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="n">
+        <v>0</v>
+      </c>
+      <c r="N147" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="n">
+        <v>0</v>
+      </c>
+      <c r="P147" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="n">
+        <v>0</v>
+      </c>
+      <c r="R147" t="n">
+        <v>0</v>
+      </c>
+      <c r="S147" t="n">
+        <v>0</v>
+      </c>
+      <c r="T147" t="n">
+        <v>0</v>
+      </c>
+      <c r="U147" t="n">
+        <v>0</v>
+      </c>
+      <c r="V147" t="n">
+        <v>0</v>
+      </c>
+      <c r="W147" t="n">
+        <v>0</v>
+      </c>
+      <c r="X147" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y147" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z147" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA147" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>201145</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Jeff Green</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>1:43</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
+        <v>1</v>
+      </c>
+      <c r="J148" t="n">
+        <v>1</v>
+      </c>
+      <c r="K148" t="n">
+        <v>1</v>
+      </c>
+      <c r="L148" t="n">
+        <v>1</v>
+      </c>
+      <c r="M148" t="n">
+        <v>1</v>
+      </c>
+      <c r="N148" t="n">
+        <v>1</v>
+      </c>
+      <c r="O148" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="n">
+        <v>0</v>
+      </c>
+      <c r="R148" t="n">
+        <v>0</v>
+      </c>
+      <c r="S148" t="n">
+        <v>0</v>
+      </c>
+      <c r="T148" t="n">
+        <v>0</v>
+      </c>
+      <c r="U148" t="n">
+        <v>0</v>
+      </c>
+      <c r="V148" t="n">
+        <v>0</v>
+      </c>
+      <c r="W148" t="n">
+        <v>0</v>
+      </c>
+      <c r="X148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z148" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA148" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>1631466</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Nate Williams</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>1:43</t>
+        </is>
+      </c>
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" t="n">
+        <v>1</v>
+      </c>
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" t="n">
+        <v>1</v>
+      </c>
+      <c r="N149" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" t="n">
+        <v>0</v>
+      </c>
+      <c r="P149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>0</v>
+      </c>
+      <c r="R149" t="n">
+        <v>0</v>
+      </c>
+      <c r="S149" t="n">
+        <v>0</v>
+      </c>
+      <c r="T149" t="n">
+        <v>0</v>
+      </c>
+      <c r="U149" t="n">
+        <v>0</v>
+      </c>
+      <c r="V149" t="n">
+        <v>0</v>
+      </c>
+      <c r="W149" t="n">
+        <v>0</v>
+      </c>
+      <c r="X149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y149" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA149" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>1641715</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Cam Whitmore</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>1:43</t>
+        </is>
+      </c>
+      <c r="I150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" t="n">
+        <v>0</v>
+      </c>
+      <c r="L150" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="n">
+        <v>0</v>
+      </c>
+      <c r="N150" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" t="n">
+        <v>0</v>
+      </c>
+      <c r="P150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>0</v>
+      </c>
+      <c r="R150" t="n">
+        <v>0</v>
+      </c>
+      <c r="S150" t="n">
+        <v>0</v>
+      </c>
+      <c r="T150" t="n">
+        <v>0</v>
+      </c>
+      <c r="U150" t="n">
+        <v>0</v>
+      </c>
+      <c r="V150" t="n">
+        <v>0</v>
+      </c>
+      <c r="W150" t="n">
+        <v>0</v>
+      </c>
+      <c r="X150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA150" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>1630256</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Jae'Sean Tate</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>0</v>
+      </c>
+      <c r="R151" t="n">
+        <v>0</v>
+      </c>
+      <c r="S151" t="n">
+        <v>0</v>
+      </c>
+      <c r="T151" t="n">
+        <v>0</v>
+      </c>
+      <c r="U151" t="n">
+        <v>0</v>
+      </c>
+      <c r="V151" t="n">
+        <v>0</v>
+      </c>
+      <c r="W151" t="n">
+        <v>0</v>
+      </c>
+      <c r="X151" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y151" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z151" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA151" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add GSW vs MIN GM1 & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA211"/>
+  <dimension ref="A1:AA240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20303,6 +20303,2729 @@
         <v>0</v>
       </c>
     </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>39:59</t>
+        </is>
+      </c>
+      <c r="I212" t="n">
+        <v>7</v>
+      </c>
+      <c r="J212" t="n">
+        <v>19</v>
+      </c>
+      <c r="K212" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="L212" t="n">
+        <v>5</v>
+      </c>
+      <c r="M212" t="n">
+        <v>8</v>
+      </c>
+      <c r="N212" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="O212" t="n">
+        <v>5</v>
+      </c>
+      <c r="P212" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q212" t="n">
+        <v>1</v>
+      </c>
+      <c r="R212" t="n">
+        <v>4</v>
+      </c>
+      <c r="S212" t="n">
+        <v>4</v>
+      </c>
+      <c r="T212" t="n">
+        <v>8</v>
+      </c>
+      <c r="U212" t="n">
+        <v>3</v>
+      </c>
+      <c r="V212" t="n">
+        <v>1</v>
+      </c>
+      <c r="W212" t="n">
+        <v>0</v>
+      </c>
+      <c r="X212" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y212" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z212" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA212" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>41:16</t>
+        </is>
+      </c>
+      <c r="I213" t="n">
+        <v>7</v>
+      </c>
+      <c r="J213" t="n">
+        <v>20</v>
+      </c>
+      <c r="K213" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="L213" t="n">
+        <v>2</v>
+      </c>
+      <c r="M213" t="n">
+        <v>8</v>
+      </c>
+      <c r="N213" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O213" t="n">
+        <v>4</v>
+      </c>
+      <c r="P213" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q213" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="R213" t="n">
+        <v>7</v>
+      </c>
+      <c r="S213" t="n">
+        <v>4</v>
+      </c>
+      <c r="T213" t="n">
+        <v>11</v>
+      </c>
+      <c r="U213" t="n">
+        <v>8</v>
+      </c>
+      <c r="V213" t="n">
+        <v>2</v>
+      </c>
+      <c r="W213" t="n">
+        <v>0</v>
+      </c>
+      <c r="X213" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y213" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z213" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA213" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>34:33</t>
+        </is>
+      </c>
+      <c r="I214" t="n">
+        <v>6</v>
+      </c>
+      <c r="J214" t="n">
+        <v>13</v>
+      </c>
+      <c r="K214" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="L214" t="n">
+        <v>4</v>
+      </c>
+      <c r="M214" t="n">
+        <v>10</v>
+      </c>
+      <c r="N214" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O214" t="n">
+        <v>2</v>
+      </c>
+      <c r="P214" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q214" t="n">
+        <v>1</v>
+      </c>
+      <c r="R214" t="n">
+        <v>0</v>
+      </c>
+      <c r="S214" t="n">
+        <v>8</v>
+      </c>
+      <c r="T214" t="n">
+        <v>8</v>
+      </c>
+      <c r="U214" t="n">
+        <v>6</v>
+      </c>
+      <c r="V214" t="n">
+        <v>2</v>
+      </c>
+      <c r="W214" t="n">
+        <v>0</v>
+      </c>
+      <c r="X214" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y214" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z214" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA214" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>29:00</t>
+        </is>
+      </c>
+      <c r="I215" t="n">
+        <v>1</v>
+      </c>
+      <c r="J215" t="n">
+        <v>7</v>
+      </c>
+      <c r="K215" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="L215" t="n">
+        <v>1</v>
+      </c>
+      <c r="M215" t="n">
+        <v>5</v>
+      </c>
+      <c r="N215" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O215" t="n">
+        <v>0</v>
+      </c>
+      <c r="P215" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q215" t="n">
+        <v>0</v>
+      </c>
+      <c r="R215" t="n">
+        <v>0</v>
+      </c>
+      <c r="S215" t="n">
+        <v>8</v>
+      </c>
+      <c r="T215" t="n">
+        <v>8</v>
+      </c>
+      <c r="U215" t="n">
+        <v>3</v>
+      </c>
+      <c r="V215" t="n">
+        <v>0</v>
+      </c>
+      <c r="W215" t="n">
+        <v>0</v>
+      </c>
+      <c r="X215" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y215" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z215" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA215" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="I216" t="n">
+        <v>5</v>
+      </c>
+      <c r="J216" t="n">
+        <v>9</v>
+      </c>
+      <c r="K216" t="n">
+        <v>0.556</v>
+      </c>
+      <c r="L216" t="n">
+        <v>3</v>
+      </c>
+      <c r="M216" t="n">
+        <v>6</v>
+      </c>
+      <c r="N216" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O216" t="n">
+        <v>0</v>
+      </c>
+      <c r="P216" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q216" t="n">
+        <v>0</v>
+      </c>
+      <c r="R216" t="n">
+        <v>0</v>
+      </c>
+      <c r="S216" t="n">
+        <v>1</v>
+      </c>
+      <c r="T216" t="n">
+        <v>1</v>
+      </c>
+      <c r="U216" t="n">
+        <v>1</v>
+      </c>
+      <c r="V216" t="n">
+        <v>0</v>
+      </c>
+      <c r="W216" t="n">
+        <v>0</v>
+      </c>
+      <c r="X216" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y216" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z216" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA216" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="I217" t="n">
+        <v>0</v>
+      </c>
+      <c r="J217" t="n">
+        <v>4</v>
+      </c>
+      <c r="K217" t="n">
+        <v>0</v>
+      </c>
+      <c r="L217" t="n">
+        <v>0</v>
+      </c>
+      <c r="M217" t="n">
+        <v>1</v>
+      </c>
+      <c r="N217" t="n">
+        <v>0</v>
+      </c>
+      <c r="O217" t="n">
+        <v>0</v>
+      </c>
+      <c r="P217" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q217" t="n">
+        <v>0</v>
+      </c>
+      <c r="R217" t="n">
+        <v>0</v>
+      </c>
+      <c r="S217" t="n">
+        <v>0</v>
+      </c>
+      <c r="T217" t="n">
+        <v>0</v>
+      </c>
+      <c r="U217" t="n">
+        <v>0</v>
+      </c>
+      <c r="V217" t="n">
+        <v>0</v>
+      </c>
+      <c r="W217" t="n">
+        <v>0</v>
+      </c>
+      <c r="X217" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y217" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z217" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA217" t="n">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>25:55</t>
+        </is>
+      </c>
+      <c r="I218" t="n">
+        <v>3</v>
+      </c>
+      <c r="J218" t="n">
+        <v>4</v>
+      </c>
+      <c r="K218" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L218" t="n">
+        <v>2</v>
+      </c>
+      <c r="M218" t="n">
+        <v>3</v>
+      </c>
+      <c r="N218" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O218" t="n">
+        <v>0</v>
+      </c>
+      <c r="P218" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q218" t="n">
+        <v>0</v>
+      </c>
+      <c r="R218" t="n">
+        <v>2</v>
+      </c>
+      <c r="S218" t="n">
+        <v>3</v>
+      </c>
+      <c r="T218" t="n">
+        <v>5</v>
+      </c>
+      <c r="U218" t="n">
+        <v>4</v>
+      </c>
+      <c r="V218" t="n">
+        <v>1</v>
+      </c>
+      <c r="W218" t="n">
+        <v>0</v>
+      </c>
+      <c r="X218" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y218" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z218" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA218" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>3:43</t>
+        </is>
+      </c>
+      <c r="I219" t="n">
+        <v>0</v>
+      </c>
+      <c r="J219" t="n">
+        <v>0</v>
+      </c>
+      <c r="K219" t="n">
+        <v>0</v>
+      </c>
+      <c r="L219" t="n">
+        <v>0</v>
+      </c>
+      <c r="M219" t="n">
+        <v>0</v>
+      </c>
+      <c r="N219" t="n">
+        <v>0</v>
+      </c>
+      <c r="O219" t="n">
+        <v>0</v>
+      </c>
+      <c r="P219" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q219" t="n">
+        <v>0</v>
+      </c>
+      <c r="R219" t="n">
+        <v>0</v>
+      </c>
+      <c r="S219" t="n">
+        <v>0</v>
+      </c>
+      <c r="T219" t="n">
+        <v>0</v>
+      </c>
+      <c r="U219" t="n">
+        <v>0</v>
+      </c>
+      <c r="V219" t="n">
+        <v>0</v>
+      </c>
+      <c r="W219" t="n">
+        <v>0</v>
+      </c>
+      <c r="X219" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y219" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z219" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA219" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="I220" t="n">
+        <v>1</v>
+      </c>
+      <c r="J220" t="n">
+        <v>2</v>
+      </c>
+      <c r="K220" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L220" t="n">
+        <v>0</v>
+      </c>
+      <c r="M220" t="n">
+        <v>0</v>
+      </c>
+      <c r="N220" t="n">
+        <v>0</v>
+      </c>
+      <c r="O220" t="n">
+        <v>0</v>
+      </c>
+      <c r="P220" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q220" t="n">
+        <v>0</v>
+      </c>
+      <c r="R220" t="n">
+        <v>2</v>
+      </c>
+      <c r="S220" t="n">
+        <v>4</v>
+      </c>
+      <c r="T220" t="n">
+        <v>6</v>
+      </c>
+      <c r="U220" t="n">
+        <v>0</v>
+      </c>
+      <c r="V220" t="n">
+        <v>2</v>
+      </c>
+      <c r="W220" t="n">
+        <v>1</v>
+      </c>
+      <c r="X220" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y220" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z220" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA220" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>6:20</t>
+        </is>
+      </c>
+      <c r="I221" t="n">
+        <v>0</v>
+      </c>
+      <c r="J221" t="n">
+        <v>0</v>
+      </c>
+      <c r="K221" t="n">
+        <v>0</v>
+      </c>
+      <c r="L221" t="n">
+        <v>0</v>
+      </c>
+      <c r="M221" t="n">
+        <v>0</v>
+      </c>
+      <c r="N221" t="n">
+        <v>0</v>
+      </c>
+      <c r="O221" t="n">
+        <v>0</v>
+      </c>
+      <c r="P221" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q221" t="n">
+        <v>0</v>
+      </c>
+      <c r="R221" t="n">
+        <v>0</v>
+      </c>
+      <c r="S221" t="n">
+        <v>1</v>
+      </c>
+      <c r="T221" t="n">
+        <v>1</v>
+      </c>
+      <c r="U221" t="n">
+        <v>0</v>
+      </c>
+      <c r="V221" t="n">
+        <v>0</v>
+      </c>
+      <c r="W221" t="n">
+        <v>0</v>
+      </c>
+      <c r="X221" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y221" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA221" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>13:10</t>
+        </is>
+      </c>
+      <c r="I222" t="n">
+        <v>2</v>
+      </c>
+      <c r="J222" t="n">
+        <v>5</v>
+      </c>
+      <c r="K222" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L222" t="n">
+        <v>1</v>
+      </c>
+      <c r="M222" t="n">
+        <v>1</v>
+      </c>
+      <c r="N222" t="n">
+        <v>1</v>
+      </c>
+      <c r="O222" t="n">
+        <v>2</v>
+      </c>
+      <c r="P222" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q222" t="n">
+        <v>1</v>
+      </c>
+      <c r="R222" t="n">
+        <v>1</v>
+      </c>
+      <c r="S222" t="n">
+        <v>0</v>
+      </c>
+      <c r="T222" t="n">
+        <v>1</v>
+      </c>
+      <c r="U222" t="n">
+        <v>1</v>
+      </c>
+      <c r="V222" t="n">
+        <v>0</v>
+      </c>
+      <c r="W222" t="n">
+        <v>1</v>
+      </c>
+      <c r="X222" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y222" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z222" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA222" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>10:33</t>
+        </is>
+      </c>
+      <c r="I223" t="n">
+        <v>2</v>
+      </c>
+      <c r="J223" t="n">
+        <v>4</v>
+      </c>
+      <c r="K223" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L223" t="n">
+        <v>0</v>
+      </c>
+      <c r="M223" t="n">
+        <v>0</v>
+      </c>
+      <c r="N223" t="n">
+        <v>0</v>
+      </c>
+      <c r="O223" t="n">
+        <v>0</v>
+      </c>
+      <c r="P223" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q223" t="n">
+        <v>0</v>
+      </c>
+      <c r="R223" t="n">
+        <v>2</v>
+      </c>
+      <c r="S223" t="n">
+        <v>0</v>
+      </c>
+      <c r="T223" t="n">
+        <v>2</v>
+      </c>
+      <c r="U223" t="n">
+        <v>0</v>
+      </c>
+      <c r="V223" t="n">
+        <v>2</v>
+      </c>
+      <c r="W223" t="n">
+        <v>0</v>
+      </c>
+      <c r="X223" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y223" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z223" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA223" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr"/>
+      <c r="I224" t="n">
+        <v>0</v>
+      </c>
+      <c r="J224" t="n">
+        <v>0</v>
+      </c>
+      <c r="K224" t="n">
+        <v>0</v>
+      </c>
+      <c r="L224" t="n">
+        <v>0</v>
+      </c>
+      <c r="M224" t="n">
+        <v>0</v>
+      </c>
+      <c r="N224" t="n">
+        <v>0</v>
+      </c>
+      <c r="O224" t="n">
+        <v>0</v>
+      </c>
+      <c r="P224" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q224" t="n">
+        <v>0</v>
+      </c>
+      <c r="R224" t="n">
+        <v>0</v>
+      </c>
+      <c r="S224" t="n">
+        <v>0</v>
+      </c>
+      <c r="T224" t="n">
+        <v>0</v>
+      </c>
+      <c r="U224" t="n">
+        <v>0</v>
+      </c>
+      <c r="V224" t="n">
+        <v>0</v>
+      </c>
+      <c r="W224" t="n">
+        <v>0</v>
+      </c>
+      <c r="X224" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y224" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA224" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr"/>
+      <c r="I225" t="n">
+        <v>0</v>
+      </c>
+      <c r="J225" t="n">
+        <v>0</v>
+      </c>
+      <c r="K225" t="n">
+        <v>0</v>
+      </c>
+      <c r="L225" t="n">
+        <v>0</v>
+      </c>
+      <c r="M225" t="n">
+        <v>0</v>
+      </c>
+      <c r="N225" t="n">
+        <v>0</v>
+      </c>
+      <c r="O225" t="n">
+        <v>0</v>
+      </c>
+      <c r="P225" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q225" t="n">
+        <v>0</v>
+      </c>
+      <c r="R225" t="n">
+        <v>0</v>
+      </c>
+      <c r="S225" t="n">
+        <v>0</v>
+      </c>
+      <c r="T225" t="n">
+        <v>0</v>
+      </c>
+      <c r="U225" t="n">
+        <v>0</v>
+      </c>
+      <c r="V225" t="n">
+        <v>0</v>
+      </c>
+      <c r="W225" t="n">
+        <v>0</v>
+      </c>
+      <c r="X225" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y225" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA225" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr"/>
+      <c r="I226" t="n">
+        <v>0</v>
+      </c>
+      <c r="J226" t="n">
+        <v>0</v>
+      </c>
+      <c r="K226" t="n">
+        <v>0</v>
+      </c>
+      <c r="L226" t="n">
+        <v>0</v>
+      </c>
+      <c r="M226" t="n">
+        <v>0</v>
+      </c>
+      <c r="N226" t="n">
+        <v>0</v>
+      </c>
+      <c r="O226" t="n">
+        <v>0</v>
+      </c>
+      <c r="P226" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q226" t="n">
+        <v>0</v>
+      </c>
+      <c r="R226" t="n">
+        <v>0</v>
+      </c>
+      <c r="S226" t="n">
+        <v>0</v>
+      </c>
+      <c r="T226" t="n">
+        <v>0</v>
+      </c>
+      <c r="U226" t="n">
+        <v>0</v>
+      </c>
+      <c r="V226" t="n">
+        <v>0</v>
+      </c>
+      <c r="W226" t="n">
+        <v>0</v>
+      </c>
+      <c r="X226" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y226" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA226" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>1630183</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Jaden McDaniels</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>37:38</t>
+        </is>
+      </c>
+      <c r="I227" t="n">
+        <v>6</v>
+      </c>
+      <c r="J227" t="n">
+        <v>12</v>
+      </c>
+      <c r="K227" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L227" t="n">
+        <v>0</v>
+      </c>
+      <c r="M227" t="n">
+        <v>3</v>
+      </c>
+      <c r="N227" t="n">
+        <v>0</v>
+      </c>
+      <c r="O227" t="n">
+        <v>0</v>
+      </c>
+      <c r="P227" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q227" t="n">
+        <v>0</v>
+      </c>
+      <c r="R227" t="n">
+        <v>3</v>
+      </c>
+      <c r="S227" t="n">
+        <v>1</v>
+      </c>
+      <c r="T227" t="n">
+        <v>4</v>
+      </c>
+      <c r="U227" t="n">
+        <v>1</v>
+      </c>
+      <c r="V227" t="n">
+        <v>0</v>
+      </c>
+      <c r="W227" t="n">
+        <v>1</v>
+      </c>
+      <c r="X227" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y227" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z227" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="n">
+        <v>203944</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Julius Randle</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>30:36</t>
+        </is>
+      </c>
+      <c r="I228" t="n">
+        <v>4</v>
+      </c>
+      <c r="J228" t="n">
+        <v>11</v>
+      </c>
+      <c r="K228" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="L228" t="n">
+        <v>0</v>
+      </c>
+      <c r="M228" t="n">
+        <v>3</v>
+      </c>
+      <c r="N228" t="n">
+        <v>0</v>
+      </c>
+      <c r="O228" t="n">
+        <v>10</v>
+      </c>
+      <c r="P228" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q228" t="n">
+        <v>1</v>
+      </c>
+      <c r="R228" t="n">
+        <v>1</v>
+      </c>
+      <c r="S228" t="n">
+        <v>2</v>
+      </c>
+      <c r="T228" t="n">
+        <v>3</v>
+      </c>
+      <c r="U228" t="n">
+        <v>6</v>
+      </c>
+      <c r="V228" t="n">
+        <v>0</v>
+      </c>
+      <c r="W228" t="n">
+        <v>0</v>
+      </c>
+      <c r="X228" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y228" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z228" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA228" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="n">
+        <v>203497</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Rudy Gobert</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>26:12</t>
+        </is>
+      </c>
+      <c r="I229" t="n">
+        <v>4</v>
+      </c>
+      <c r="J229" t="n">
+        <v>7</v>
+      </c>
+      <c r="K229" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="L229" t="n">
+        <v>0</v>
+      </c>
+      <c r="M229" t="n">
+        <v>0</v>
+      </c>
+      <c r="N229" t="n">
+        <v>0</v>
+      </c>
+      <c r="O229" t="n">
+        <v>1</v>
+      </c>
+      <c r="P229" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q229" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R229" t="n">
+        <v>4</v>
+      </c>
+      <c r="S229" t="n">
+        <v>7</v>
+      </c>
+      <c r="T229" t="n">
+        <v>11</v>
+      </c>
+      <c r="U229" t="n">
+        <v>0</v>
+      </c>
+      <c r="V229" t="n">
+        <v>0</v>
+      </c>
+      <c r="W229" t="n">
+        <v>3</v>
+      </c>
+      <c r="X229" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y229" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z229" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA229" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="n">
+        <v>1630162</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Anthony Edwards</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>41:44</t>
+        </is>
+      </c>
+      <c r="I230" t="n">
+        <v>9</v>
+      </c>
+      <c r="J230" t="n">
+        <v>22</v>
+      </c>
+      <c r="K230" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="L230" t="n">
+        <v>1</v>
+      </c>
+      <c r="M230" t="n">
+        <v>5</v>
+      </c>
+      <c r="N230" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O230" t="n">
+        <v>4</v>
+      </c>
+      <c r="P230" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q230" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R230" t="n">
+        <v>1</v>
+      </c>
+      <c r="S230" t="n">
+        <v>13</v>
+      </c>
+      <c r="T230" t="n">
+        <v>14</v>
+      </c>
+      <c r="U230" t="n">
+        <v>2</v>
+      </c>
+      <c r="V230" t="n">
+        <v>3</v>
+      </c>
+      <c r="W230" t="n">
+        <v>1</v>
+      </c>
+      <c r="X230" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y230" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z230" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA230" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="n">
+        <v>201144</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Mike Conley</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>21:44</t>
+        </is>
+      </c>
+      <c r="I231" t="n">
+        <v>0</v>
+      </c>
+      <c r="J231" t="n">
+        <v>5</v>
+      </c>
+      <c r="K231" t="n">
+        <v>0</v>
+      </c>
+      <c r="L231" t="n">
+        <v>0</v>
+      </c>
+      <c r="M231" t="n">
+        <v>2</v>
+      </c>
+      <c r="N231" t="n">
+        <v>0</v>
+      </c>
+      <c r="O231" t="n">
+        <v>0</v>
+      </c>
+      <c r="P231" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q231" t="n">
+        <v>0</v>
+      </c>
+      <c r="R231" t="n">
+        <v>0</v>
+      </c>
+      <c r="S231" t="n">
+        <v>1</v>
+      </c>
+      <c r="T231" t="n">
+        <v>1</v>
+      </c>
+      <c r="U231" t="n">
+        <v>5</v>
+      </c>
+      <c r="V231" t="n">
+        <v>1</v>
+      </c>
+      <c r="W231" t="n">
+        <v>0</v>
+      </c>
+      <c r="X231" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y231" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z231" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA231" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="n">
+        <v>1628978</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Donte DiVincenzo</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>32:32</t>
+        </is>
+      </c>
+      <c r="I232" t="n">
+        <v>3</v>
+      </c>
+      <c r="J232" t="n">
+        <v>11</v>
+      </c>
+      <c r="K232" t="n">
+        <v>0.273</v>
+      </c>
+      <c r="L232" t="n">
+        <v>1</v>
+      </c>
+      <c r="M232" t="n">
+        <v>7</v>
+      </c>
+      <c r="N232" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="O232" t="n">
+        <v>0</v>
+      </c>
+      <c r="P232" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q232" t="n">
+        <v>0</v>
+      </c>
+      <c r="R232" t="n">
+        <v>1</v>
+      </c>
+      <c r="S232" t="n">
+        <v>2</v>
+      </c>
+      <c r="T232" t="n">
+        <v>3</v>
+      </c>
+      <c r="U232" t="n">
+        <v>4</v>
+      </c>
+      <c r="V232" t="n">
+        <v>1</v>
+      </c>
+      <c r="W232" t="n">
+        <v>0</v>
+      </c>
+      <c r="X232" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y232" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z232" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA232" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="n">
+        <v>1629675</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Naz Reid</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>33:40</t>
+        </is>
+      </c>
+      <c r="I233" t="n">
+        <v>8</v>
+      </c>
+      <c r="J233" t="n">
+        <v>14</v>
+      </c>
+      <c r="K233" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="L233" t="n">
+        <v>3</v>
+      </c>
+      <c r="M233" t="n">
+        <v>7</v>
+      </c>
+      <c r="N233" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="O233" t="n">
+        <v>0</v>
+      </c>
+      <c r="P233" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q233" t="n">
+        <v>0</v>
+      </c>
+      <c r="R233" t="n">
+        <v>2</v>
+      </c>
+      <c r="S233" t="n">
+        <v>3</v>
+      </c>
+      <c r="T233" t="n">
+        <v>5</v>
+      </c>
+      <c r="U233" t="n">
+        <v>1</v>
+      </c>
+      <c r="V233" t="n">
+        <v>1</v>
+      </c>
+      <c r="W233" t="n">
+        <v>1</v>
+      </c>
+      <c r="X233" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y233" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z233" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA233" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="n">
+        <v>1629638</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>14:08</t>
+        </is>
+      </c>
+      <c r="I234" t="n">
+        <v>0</v>
+      </c>
+      <c r="J234" t="n">
+        <v>3</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0</v>
+      </c>
+      <c r="L234" t="n">
+        <v>0</v>
+      </c>
+      <c r="M234" t="n">
+        <v>2</v>
+      </c>
+      <c r="N234" t="n">
+        <v>0</v>
+      </c>
+      <c r="O234" t="n">
+        <v>0</v>
+      </c>
+      <c r="P234" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q234" t="n">
+        <v>0</v>
+      </c>
+      <c r="R234" t="n">
+        <v>0</v>
+      </c>
+      <c r="S234" t="n">
+        <v>0</v>
+      </c>
+      <c r="T234" t="n">
+        <v>0</v>
+      </c>
+      <c r="U234" t="n">
+        <v>0</v>
+      </c>
+      <c r="V234" t="n">
+        <v>1</v>
+      </c>
+      <c r="W234" t="n">
+        <v>0</v>
+      </c>
+      <c r="X234" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y234" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA234" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="n">
+        <v>1630545</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Terrence Shannon Jr.</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>1:46</t>
+        </is>
+      </c>
+      <c r="I235" t="n">
+        <v>0</v>
+      </c>
+      <c r="J235" t="n">
+        <v>1</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0</v>
+      </c>
+      <c r="L235" t="n">
+        <v>0</v>
+      </c>
+      <c r="M235" t="n">
+        <v>0</v>
+      </c>
+      <c r="N235" t="n">
+        <v>0</v>
+      </c>
+      <c r="O235" t="n">
+        <v>0</v>
+      </c>
+      <c r="P235" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q235" t="n">
+        <v>0</v>
+      </c>
+      <c r="R235" t="n">
+        <v>0</v>
+      </c>
+      <c r="S235" t="n">
+        <v>0</v>
+      </c>
+      <c r="T235" t="n">
+        <v>0</v>
+      </c>
+      <c r="U235" t="n">
+        <v>0</v>
+      </c>
+      <c r="V235" t="n">
+        <v>0</v>
+      </c>
+      <c r="W235" t="n">
+        <v>0</v>
+      </c>
+      <c r="X235" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y235" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z235" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA235" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="n">
+        <v>1641740</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Jaylen Clark</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr"/>
+      <c r="I236" t="n">
+        <v>0</v>
+      </c>
+      <c r="J236" t="n">
+        <v>0</v>
+      </c>
+      <c r="K236" t="n">
+        <v>0</v>
+      </c>
+      <c r="L236" t="n">
+        <v>0</v>
+      </c>
+      <c r="M236" t="n">
+        <v>0</v>
+      </c>
+      <c r="N236" t="n">
+        <v>0</v>
+      </c>
+      <c r="O236" t="n">
+        <v>0</v>
+      </c>
+      <c r="P236" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q236" t="n">
+        <v>0</v>
+      </c>
+      <c r="R236" t="n">
+        <v>0</v>
+      </c>
+      <c r="S236" t="n">
+        <v>0</v>
+      </c>
+      <c r="T236" t="n">
+        <v>0</v>
+      </c>
+      <c r="U236" t="n">
+        <v>0</v>
+      </c>
+      <c r="V236" t="n">
+        <v>0</v>
+      </c>
+      <c r="W236" t="n">
+        <v>0</v>
+      </c>
+      <c r="X236" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y236" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z236" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="n">
+        <v>1630568</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Luka Garza</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr"/>
+      <c r="I237" t="n">
+        <v>0</v>
+      </c>
+      <c r="J237" t="n">
+        <v>0</v>
+      </c>
+      <c r="K237" t="n">
+        <v>0</v>
+      </c>
+      <c r="L237" t="n">
+        <v>0</v>
+      </c>
+      <c r="M237" t="n">
+        <v>0</v>
+      </c>
+      <c r="N237" t="n">
+        <v>0</v>
+      </c>
+      <c r="O237" t="n">
+        <v>0</v>
+      </c>
+      <c r="P237" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q237" t="n">
+        <v>0</v>
+      </c>
+      <c r="R237" t="n">
+        <v>0</v>
+      </c>
+      <c r="S237" t="n">
+        <v>0</v>
+      </c>
+      <c r="T237" t="n">
+        <v>0</v>
+      </c>
+      <c r="U237" t="n">
+        <v>0</v>
+      </c>
+      <c r="V237" t="n">
+        <v>0</v>
+      </c>
+      <c r="W237" t="n">
+        <v>0</v>
+      </c>
+      <c r="X237" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y237" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z237" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="n">
+        <v>204060</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Joe Ingles</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr"/>
+      <c r="I238" t="n">
+        <v>0</v>
+      </c>
+      <c r="J238" t="n">
+        <v>0</v>
+      </c>
+      <c r="K238" t="n">
+        <v>0</v>
+      </c>
+      <c r="L238" t="n">
+        <v>0</v>
+      </c>
+      <c r="M238" t="n">
+        <v>0</v>
+      </c>
+      <c r="N238" t="n">
+        <v>0</v>
+      </c>
+      <c r="O238" t="n">
+        <v>0</v>
+      </c>
+      <c r="P238" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q238" t="n">
+        <v>0</v>
+      </c>
+      <c r="R238" t="n">
+        <v>0</v>
+      </c>
+      <c r="S238" t="n">
+        <v>0</v>
+      </c>
+      <c r="T238" t="n">
+        <v>0</v>
+      </c>
+      <c r="U238" t="n">
+        <v>0</v>
+      </c>
+      <c r="V238" t="n">
+        <v>0</v>
+      </c>
+      <c r="W238" t="n">
+        <v>0</v>
+      </c>
+      <c r="X238" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y238" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z238" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="n">
+        <v>1631159</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Leonard Miller</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr"/>
+      <c r="I239" t="n">
+        <v>0</v>
+      </c>
+      <c r="J239" t="n">
+        <v>0</v>
+      </c>
+      <c r="K239" t="n">
+        <v>0</v>
+      </c>
+      <c r="L239" t="n">
+        <v>0</v>
+      </c>
+      <c r="M239" t="n">
+        <v>0</v>
+      </c>
+      <c r="N239" t="n">
+        <v>0</v>
+      </c>
+      <c r="O239" t="n">
+        <v>0</v>
+      </c>
+      <c r="P239" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q239" t="n">
+        <v>0</v>
+      </c>
+      <c r="R239" t="n">
+        <v>0</v>
+      </c>
+      <c r="S239" t="n">
+        <v>0</v>
+      </c>
+      <c r="T239" t="n">
+        <v>0</v>
+      </c>
+      <c r="U239" t="n">
+        <v>0</v>
+      </c>
+      <c r="V239" t="n">
+        <v>0</v>
+      </c>
+      <c r="W239" t="n">
+        <v>0</v>
+      </c>
+      <c r="X239" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y239" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="n">
+        <v>1631169</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Josh Minott</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr"/>
+      <c r="I240" t="n">
+        <v>0</v>
+      </c>
+      <c r="J240" t="n">
+        <v>0</v>
+      </c>
+      <c r="K240" t="n">
+        <v>0</v>
+      </c>
+      <c r="L240" t="n">
+        <v>0</v>
+      </c>
+      <c r="M240" t="n">
+        <v>0</v>
+      </c>
+      <c r="N240" t="n">
+        <v>0</v>
+      </c>
+      <c r="O240" t="n">
+        <v>0</v>
+      </c>
+      <c r="P240" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q240" t="n">
+        <v>0</v>
+      </c>
+      <c r="R240" t="n">
+        <v>0</v>
+      </c>
+      <c r="S240" t="n">
+        <v>0</v>
+      </c>
+      <c r="T240" t="n">
+        <v>0</v>
+      </c>
+      <c r="U240" t="n">
+        <v>0</v>
+      </c>
+      <c r="V240" t="n">
+        <v>0</v>
+      </c>
+      <c r="W240" t="n">
+        <v>0</v>
+      </c>
+      <c r="X240" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y240" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA240" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add GSW vs MIN GM2 & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA240"/>
+  <dimension ref="A1:AA269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23026,6 +23026,2753 @@
         <v>0</v>
       </c>
     </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>33:51</t>
+        </is>
+      </c>
+      <c r="I241" t="n">
+        <v>6</v>
+      </c>
+      <c r="J241" t="n">
+        <v>13</v>
+      </c>
+      <c r="K241" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="L241" t="n">
+        <v>2</v>
+      </c>
+      <c r="M241" t="n">
+        <v>4</v>
+      </c>
+      <c r="N241" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O241" t="n">
+        <v>3</v>
+      </c>
+      <c r="P241" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q241" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="R241" t="n">
+        <v>2</v>
+      </c>
+      <c r="S241" t="n">
+        <v>5</v>
+      </c>
+      <c r="T241" t="n">
+        <v>7</v>
+      </c>
+      <c r="U241" t="n">
+        <v>4</v>
+      </c>
+      <c r="V241" t="n">
+        <v>1</v>
+      </c>
+      <c r="W241" t="n">
+        <v>0</v>
+      </c>
+      <c r="X241" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y241" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z241" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA241" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>29:09</t>
+        </is>
+      </c>
+      <c r="I242" t="n">
+        <v>3</v>
+      </c>
+      <c r="J242" t="n">
+        <v>10</v>
+      </c>
+      <c r="K242" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L242" t="n">
+        <v>1</v>
+      </c>
+      <c r="M242" t="n">
+        <v>6</v>
+      </c>
+      <c r="N242" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="O242" t="n">
+        <v>2</v>
+      </c>
+      <c r="P242" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q242" t="n">
+        <v>1</v>
+      </c>
+      <c r="R242" t="n">
+        <v>0</v>
+      </c>
+      <c r="S242" t="n">
+        <v>4</v>
+      </c>
+      <c r="T242" t="n">
+        <v>4</v>
+      </c>
+      <c r="U242" t="n">
+        <v>5</v>
+      </c>
+      <c r="V242" t="n">
+        <v>1</v>
+      </c>
+      <c r="W242" t="n">
+        <v>1</v>
+      </c>
+      <c r="X242" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y242" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z242" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA242" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>3:18</t>
+        </is>
+      </c>
+      <c r="I243" t="n">
+        <v>0</v>
+      </c>
+      <c r="J243" t="n">
+        <v>0</v>
+      </c>
+      <c r="K243" t="n">
+        <v>0</v>
+      </c>
+      <c r="L243" t="n">
+        <v>0</v>
+      </c>
+      <c r="M243" t="n">
+        <v>0</v>
+      </c>
+      <c r="N243" t="n">
+        <v>0</v>
+      </c>
+      <c r="O243" t="n">
+        <v>0</v>
+      </c>
+      <c r="P243" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q243" t="n">
+        <v>0</v>
+      </c>
+      <c r="R243" t="n">
+        <v>0</v>
+      </c>
+      <c r="S243" t="n">
+        <v>0</v>
+      </c>
+      <c r="T243" t="n">
+        <v>0</v>
+      </c>
+      <c r="U243" t="n">
+        <v>0</v>
+      </c>
+      <c r="V243" t="n">
+        <v>0</v>
+      </c>
+      <c r="W243" t="n">
+        <v>0</v>
+      </c>
+      <c r="X243" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y243" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z243" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA243" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>28:39</t>
+        </is>
+      </c>
+      <c r="I244" t="n">
+        <v>5</v>
+      </c>
+      <c r="J244" t="n">
+        <v>14</v>
+      </c>
+      <c r="K244" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="L244" t="n">
+        <v>4</v>
+      </c>
+      <c r="M244" t="n">
+        <v>9</v>
+      </c>
+      <c r="N244" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="O244" t="n">
+        <v>1</v>
+      </c>
+      <c r="P244" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q244" t="n">
+        <v>1</v>
+      </c>
+      <c r="R244" t="n">
+        <v>1</v>
+      </c>
+      <c r="S244" t="n">
+        <v>2</v>
+      </c>
+      <c r="T244" t="n">
+        <v>3</v>
+      </c>
+      <c r="U244" t="n">
+        <v>1</v>
+      </c>
+      <c r="V244" t="n">
+        <v>1</v>
+      </c>
+      <c r="W244" t="n">
+        <v>0</v>
+      </c>
+      <c r="X244" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y244" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z244" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA244" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>33:02</t>
+        </is>
+      </c>
+      <c r="I245" t="n">
+        <v>4</v>
+      </c>
+      <c r="J245" t="n">
+        <v>9</v>
+      </c>
+      <c r="K245" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="L245" t="n">
+        <v>1</v>
+      </c>
+      <c r="M245" t="n">
+        <v>4</v>
+      </c>
+      <c r="N245" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O245" t="n">
+        <v>2</v>
+      </c>
+      <c r="P245" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q245" t="n">
+        <v>1</v>
+      </c>
+      <c r="R245" t="n">
+        <v>2</v>
+      </c>
+      <c r="S245" t="n">
+        <v>4</v>
+      </c>
+      <c r="T245" t="n">
+        <v>6</v>
+      </c>
+      <c r="U245" t="n">
+        <v>6</v>
+      </c>
+      <c r="V245" t="n">
+        <v>2</v>
+      </c>
+      <c r="W245" t="n">
+        <v>0</v>
+      </c>
+      <c r="X245" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y245" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z245" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA245" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>11:16</t>
+        </is>
+      </c>
+      <c r="I246" t="n">
+        <v>0</v>
+      </c>
+      <c r="J246" t="n">
+        <v>2</v>
+      </c>
+      <c r="K246" t="n">
+        <v>0</v>
+      </c>
+      <c r="L246" t="n">
+        <v>0</v>
+      </c>
+      <c r="M246" t="n">
+        <v>1</v>
+      </c>
+      <c r="N246" t="n">
+        <v>0</v>
+      </c>
+      <c r="O246" t="n">
+        <v>0</v>
+      </c>
+      <c r="P246" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q246" t="n">
+        <v>0</v>
+      </c>
+      <c r="R246" t="n">
+        <v>1</v>
+      </c>
+      <c r="S246" t="n">
+        <v>0</v>
+      </c>
+      <c r="T246" t="n">
+        <v>1</v>
+      </c>
+      <c r="U246" t="n">
+        <v>0</v>
+      </c>
+      <c r="V246" t="n">
+        <v>1</v>
+      </c>
+      <c r="W246" t="n">
+        <v>0</v>
+      </c>
+      <c r="X246" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y246" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z246" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA246" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="I247" t="n">
+        <v>0</v>
+      </c>
+      <c r="J247" t="n">
+        <v>5</v>
+      </c>
+      <c r="K247" t="n">
+        <v>0</v>
+      </c>
+      <c r="L247" t="n">
+        <v>0</v>
+      </c>
+      <c r="M247" t="n">
+        <v>4</v>
+      </c>
+      <c r="N247" t="n">
+        <v>0</v>
+      </c>
+      <c r="O247" t="n">
+        <v>3</v>
+      </c>
+      <c r="P247" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q247" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R247" t="n">
+        <v>0</v>
+      </c>
+      <c r="S247" t="n">
+        <v>2</v>
+      </c>
+      <c r="T247" t="n">
+        <v>2</v>
+      </c>
+      <c r="U247" t="n">
+        <v>1</v>
+      </c>
+      <c r="V247" t="n">
+        <v>0</v>
+      </c>
+      <c r="W247" t="n">
+        <v>0</v>
+      </c>
+      <c r="X247" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y247" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z247" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA247" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>26:23</t>
+        </is>
+      </c>
+      <c r="I248" t="n">
+        <v>8</v>
+      </c>
+      <c r="J248" t="n">
+        <v>11</v>
+      </c>
+      <c r="K248" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="L248" t="n">
+        <v>1</v>
+      </c>
+      <c r="M248" t="n">
+        <v>3</v>
+      </c>
+      <c r="N248" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O248" t="n">
+        <v>1</v>
+      </c>
+      <c r="P248" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q248" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R248" t="n">
+        <v>1</v>
+      </c>
+      <c r="S248" t="n">
+        <v>4</v>
+      </c>
+      <c r="T248" t="n">
+        <v>5</v>
+      </c>
+      <c r="U248" t="n">
+        <v>1</v>
+      </c>
+      <c r="V248" t="n">
+        <v>0</v>
+      </c>
+      <c r="W248" t="n">
+        <v>0</v>
+      </c>
+      <c r="X248" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y248" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z248" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA248" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>2:48</t>
+        </is>
+      </c>
+      <c r="I249" t="n">
+        <v>0</v>
+      </c>
+      <c r="J249" t="n">
+        <v>0</v>
+      </c>
+      <c r="K249" t="n">
+        <v>0</v>
+      </c>
+      <c r="L249" t="n">
+        <v>0</v>
+      </c>
+      <c r="M249" t="n">
+        <v>0</v>
+      </c>
+      <c r="N249" t="n">
+        <v>0</v>
+      </c>
+      <c r="O249" t="n">
+        <v>0</v>
+      </c>
+      <c r="P249" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q249" t="n">
+        <v>0</v>
+      </c>
+      <c r="R249" t="n">
+        <v>0</v>
+      </c>
+      <c r="S249" t="n">
+        <v>0</v>
+      </c>
+      <c r="T249" t="n">
+        <v>0</v>
+      </c>
+      <c r="U249" t="n">
+        <v>0</v>
+      </c>
+      <c r="V249" t="n">
+        <v>0</v>
+      </c>
+      <c r="W249" t="n">
+        <v>0</v>
+      </c>
+      <c r="X249" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y249" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z249" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA249" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="I250" t="n">
+        <v>0</v>
+      </c>
+      <c r="J250" t="n">
+        <v>2</v>
+      </c>
+      <c r="K250" t="n">
+        <v>0</v>
+      </c>
+      <c r="L250" t="n">
+        <v>0</v>
+      </c>
+      <c r="M250" t="n">
+        <v>0</v>
+      </c>
+      <c r="N250" t="n">
+        <v>0</v>
+      </c>
+      <c r="O250" t="n">
+        <v>0</v>
+      </c>
+      <c r="P250" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q250" t="n">
+        <v>0</v>
+      </c>
+      <c r="R250" t="n">
+        <v>0</v>
+      </c>
+      <c r="S250" t="n">
+        <v>2</v>
+      </c>
+      <c r="T250" t="n">
+        <v>2</v>
+      </c>
+      <c r="U250" t="n">
+        <v>1</v>
+      </c>
+      <c r="V250" t="n">
+        <v>0</v>
+      </c>
+      <c r="W250" t="n">
+        <v>0</v>
+      </c>
+      <c r="X250" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y250" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z250" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA250" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>8:29</t>
+        </is>
+      </c>
+      <c r="I251" t="n">
+        <v>0</v>
+      </c>
+      <c r="J251" t="n">
+        <v>0</v>
+      </c>
+      <c r="K251" t="n">
+        <v>0</v>
+      </c>
+      <c r="L251" t="n">
+        <v>0</v>
+      </c>
+      <c r="M251" t="n">
+        <v>0</v>
+      </c>
+      <c r="N251" t="n">
+        <v>0</v>
+      </c>
+      <c r="O251" t="n">
+        <v>0</v>
+      </c>
+      <c r="P251" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q251" t="n">
+        <v>0</v>
+      </c>
+      <c r="R251" t="n">
+        <v>0</v>
+      </c>
+      <c r="S251" t="n">
+        <v>2</v>
+      </c>
+      <c r="T251" t="n">
+        <v>2</v>
+      </c>
+      <c r="U251" t="n">
+        <v>2</v>
+      </c>
+      <c r="V251" t="n">
+        <v>1</v>
+      </c>
+      <c r="W251" t="n">
+        <v>0</v>
+      </c>
+      <c r="X251" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y251" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z251" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA251" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>9:02</t>
+        </is>
+      </c>
+      <c r="I252" t="n">
+        <v>1</v>
+      </c>
+      <c r="J252" t="n">
+        <v>3</v>
+      </c>
+      <c r="K252" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L252" t="n">
+        <v>0</v>
+      </c>
+      <c r="M252" t="n">
+        <v>1</v>
+      </c>
+      <c r="N252" t="n">
+        <v>0</v>
+      </c>
+      <c r="O252" t="n">
+        <v>1</v>
+      </c>
+      <c r="P252" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q252" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R252" t="n">
+        <v>1</v>
+      </c>
+      <c r="S252" t="n">
+        <v>1</v>
+      </c>
+      <c r="T252" t="n">
+        <v>2</v>
+      </c>
+      <c r="U252" t="n">
+        <v>0</v>
+      </c>
+      <c r="V252" t="n">
+        <v>0</v>
+      </c>
+      <c r="W252" t="n">
+        <v>0</v>
+      </c>
+      <c r="X252" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y252" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z252" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA252" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>19:18</t>
+        </is>
+      </c>
+      <c r="I253" t="n">
+        <v>6</v>
+      </c>
+      <c r="J253" t="n">
+        <v>6</v>
+      </c>
+      <c r="K253" t="n">
+        <v>1</v>
+      </c>
+      <c r="L253" t="n">
+        <v>0</v>
+      </c>
+      <c r="M253" t="n">
+        <v>0</v>
+      </c>
+      <c r="N253" t="n">
+        <v>0</v>
+      </c>
+      <c r="O253" t="n">
+        <v>3</v>
+      </c>
+      <c r="P253" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q253" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="R253" t="n">
+        <v>2</v>
+      </c>
+      <c r="S253" t="n">
+        <v>4</v>
+      </c>
+      <c r="T253" t="n">
+        <v>6</v>
+      </c>
+      <c r="U253" t="n">
+        <v>1</v>
+      </c>
+      <c r="V253" t="n">
+        <v>1</v>
+      </c>
+      <c r="W253" t="n">
+        <v>1</v>
+      </c>
+      <c r="X253" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y253" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z253" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA253" t="n">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>4:25</t>
+        </is>
+      </c>
+      <c r="I254" t="n">
+        <v>1</v>
+      </c>
+      <c r="J254" t="n">
+        <v>1</v>
+      </c>
+      <c r="K254" t="n">
+        <v>1</v>
+      </c>
+      <c r="L254" t="n">
+        <v>0</v>
+      </c>
+      <c r="M254" t="n">
+        <v>0</v>
+      </c>
+      <c r="N254" t="n">
+        <v>0</v>
+      </c>
+      <c r="O254" t="n">
+        <v>0</v>
+      </c>
+      <c r="P254" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q254" t="n">
+        <v>0</v>
+      </c>
+      <c r="R254" t="n">
+        <v>0</v>
+      </c>
+      <c r="S254" t="n">
+        <v>2</v>
+      </c>
+      <c r="T254" t="n">
+        <v>2</v>
+      </c>
+      <c r="U254" t="n">
+        <v>1</v>
+      </c>
+      <c r="V254" t="n">
+        <v>0</v>
+      </c>
+      <c r="W254" t="n">
+        <v>0</v>
+      </c>
+      <c r="X254" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y254" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z254" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA254" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr"/>
+      <c r="I255" t="n">
+        <v>0</v>
+      </c>
+      <c r="J255" t="n">
+        <v>0</v>
+      </c>
+      <c r="K255" t="n">
+        <v>0</v>
+      </c>
+      <c r="L255" t="n">
+        <v>0</v>
+      </c>
+      <c r="M255" t="n">
+        <v>0</v>
+      </c>
+      <c r="N255" t="n">
+        <v>0</v>
+      </c>
+      <c r="O255" t="n">
+        <v>0</v>
+      </c>
+      <c r="P255" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q255" t="n">
+        <v>0</v>
+      </c>
+      <c r="R255" t="n">
+        <v>0</v>
+      </c>
+      <c r="S255" t="n">
+        <v>0</v>
+      </c>
+      <c r="T255" t="n">
+        <v>0</v>
+      </c>
+      <c r="U255" t="n">
+        <v>0</v>
+      </c>
+      <c r="V255" t="n">
+        <v>0</v>
+      </c>
+      <c r="W255" t="n">
+        <v>0</v>
+      </c>
+      <c r="X255" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y255" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z255" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>1630183</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Jaden McDaniels</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>33:03</t>
+        </is>
+      </c>
+      <c r="I256" t="n">
+        <v>7</v>
+      </c>
+      <c r="J256" t="n">
+        <v>10</v>
+      </c>
+      <c r="K256" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L256" t="n">
+        <v>1</v>
+      </c>
+      <c r="M256" t="n">
+        <v>2</v>
+      </c>
+      <c r="N256" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O256" t="n">
+        <v>1</v>
+      </c>
+      <c r="P256" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q256" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R256" t="n">
+        <v>1</v>
+      </c>
+      <c r="S256" t="n">
+        <v>1</v>
+      </c>
+      <c r="T256" t="n">
+        <v>2</v>
+      </c>
+      <c r="U256" t="n">
+        <v>0</v>
+      </c>
+      <c r="V256" t="n">
+        <v>3</v>
+      </c>
+      <c r="W256" t="n">
+        <v>3</v>
+      </c>
+      <c r="X256" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y256" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z256" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA256" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>203944</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Julius Randle</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>32:54</t>
+        </is>
+      </c>
+      <c r="I257" t="n">
+        <v>10</v>
+      </c>
+      <c r="J257" t="n">
+        <v>17</v>
+      </c>
+      <c r="K257" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="L257" t="n">
+        <v>1</v>
+      </c>
+      <c r="M257" t="n">
+        <v>4</v>
+      </c>
+      <c r="N257" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O257" t="n">
+        <v>3</v>
+      </c>
+      <c r="P257" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q257" t="n">
+        <v>1</v>
+      </c>
+      <c r="R257" t="n">
+        <v>2</v>
+      </c>
+      <c r="S257" t="n">
+        <v>5</v>
+      </c>
+      <c r="T257" t="n">
+        <v>7</v>
+      </c>
+      <c r="U257" t="n">
+        <v>11</v>
+      </c>
+      <c r="V257" t="n">
+        <v>0</v>
+      </c>
+      <c r="W257" t="n">
+        <v>0</v>
+      </c>
+      <c r="X257" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y257" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z257" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA257" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>203497</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Rudy Gobert</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>26:49</t>
+        </is>
+      </c>
+      <c r="I258" t="n">
+        <v>2</v>
+      </c>
+      <c r="J258" t="n">
+        <v>4</v>
+      </c>
+      <c r="K258" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L258" t="n">
+        <v>0</v>
+      </c>
+      <c r="M258" t="n">
+        <v>0</v>
+      </c>
+      <c r="N258" t="n">
+        <v>0</v>
+      </c>
+      <c r="O258" t="n">
+        <v>1</v>
+      </c>
+      <c r="P258" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q258" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R258" t="n">
+        <v>2</v>
+      </c>
+      <c r="S258" t="n">
+        <v>7</v>
+      </c>
+      <c r="T258" t="n">
+        <v>9</v>
+      </c>
+      <c r="U258" t="n">
+        <v>0</v>
+      </c>
+      <c r="V258" t="n">
+        <v>0</v>
+      </c>
+      <c r="W258" t="n">
+        <v>0</v>
+      </c>
+      <c r="X258" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y258" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z258" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA258" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>1630162</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Anthony Edwards</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>33:54</t>
+        </is>
+      </c>
+      <c r="I259" t="n">
+        <v>6</v>
+      </c>
+      <c r="J259" t="n">
+        <v>13</v>
+      </c>
+      <c r="K259" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="L259" t="n">
+        <v>2</v>
+      </c>
+      <c r="M259" t="n">
+        <v>4</v>
+      </c>
+      <c r="N259" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O259" t="n">
+        <v>6</v>
+      </c>
+      <c r="P259" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q259" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R259" t="n">
+        <v>0</v>
+      </c>
+      <c r="S259" t="n">
+        <v>9</v>
+      </c>
+      <c r="T259" t="n">
+        <v>9</v>
+      </c>
+      <c r="U259" t="n">
+        <v>5</v>
+      </c>
+      <c r="V259" t="n">
+        <v>3</v>
+      </c>
+      <c r="W259" t="n">
+        <v>1</v>
+      </c>
+      <c r="X259" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y259" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z259" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA259" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>201144</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Mike Conley</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>17:19</t>
+        </is>
+      </c>
+      <c r="I260" t="n">
+        <v>2</v>
+      </c>
+      <c r="J260" t="n">
+        <v>5</v>
+      </c>
+      <c r="K260" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L260" t="n">
+        <v>2</v>
+      </c>
+      <c r="M260" t="n">
+        <v>4</v>
+      </c>
+      <c r="N260" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O260" t="n">
+        <v>0</v>
+      </c>
+      <c r="P260" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q260" t="n">
+        <v>0</v>
+      </c>
+      <c r="R260" t="n">
+        <v>1</v>
+      </c>
+      <c r="S260" t="n">
+        <v>1</v>
+      </c>
+      <c r="T260" t="n">
+        <v>2</v>
+      </c>
+      <c r="U260" t="n">
+        <v>2</v>
+      </c>
+      <c r="V260" t="n">
+        <v>0</v>
+      </c>
+      <c r="W260" t="n">
+        <v>0</v>
+      </c>
+      <c r="X260" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y260" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z260" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA260" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>1628978</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Donte DiVincenzo</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>25:34</t>
+        </is>
+      </c>
+      <c r="I261" t="n">
+        <v>3</v>
+      </c>
+      <c r="J261" t="n">
+        <v>9</v>
+      </c>
+      <c r="K261" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L261" t="n">
+        <v>3</v>
+      </c>
+      <c r="M261" t="n">
+        <v>8</v>
+      </c>
+      <c r="N261" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="O261" t="n">
+        <v>0</v>
+      </c>
+      <c r="P261" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q261" t="n">
+        <v>0</v>
+      </c>
+      <c r="R261" t="n">
+        <v>3</v>
+      </c>
+      <c r="S261" t="n">
+        <v>0</v>
+      </c>
+      <c r="T261" t="n">
+        <v>3</v>
+      </c>
+      <c r="U261" t="n">
+        <v>5</v>
+      </c>
+      <c r="V261" t="n">
+        <v>1</v>
+      </c>
+      <c r="W261" t="n">
+        <v>0</v>
+      </c>
+      <c r="X261" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y261" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z261" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA261" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>1629675</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Naz Reid</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>29:35</t>
+        </is>
+      </c>
+      <c r="I262" t="n">
+        <v>4</v>
+      </c>
+      <c r="J262" t="n">
+        <v>10</v>
+      </c>
+      <c r="K262" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L262" t="n">
+        <v>3</v>
+      </c>
+      <c r="M262" t="n">
+        <v>8</v>
+      </c>
+      <c r="N262" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="O262" t="n">
+        <v>0</v>
+      </c>
+      <c r="P262" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q262" t="n">
+        <v>0</v>
+      </c>
+      <c r="R262" t="n">
+        <v>0</v>
+      </c>
+      <c r="S262" t="n">
+        <v>3</v>
+      </c>
+      <c r="T262" t="n">
+        <v>3</v>
+      </c>
+      <c r="U262" t="n">
+        <v>5</v>
+      </c>
+      <c r="V262" t="n">
+        <v>1</v>
+      </c>
+      <c r="W262" t="n">
+        <v>0</v>
+      </c>
+      <c r="X262" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y262" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z262" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA262" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>1629638</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>25:37</t>
+        </is>
+      </c>
+      <c r="I263" t="n">
+        <v>7</v>
+      </c>
+      <c r="J263" t="n">
+        <v>13</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="L263" t="n">
+        <v>4</v>
+      </c>
+      <c r="M263" t="n">
+        <v>6</v>
+      </c>
+      <c r="N263" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O263" t="n">
+        <v>2</v>
+      </c>
+      <c r="P263" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q263" t="n">
+        <v>1</v>
+      </c>
+      <c r="R263" t="n">
+        <v>1</v>
+      </c>
+      <c r="S263" t="n">
+        <v>1</v>
+      </c>
+      <c r="T263" t="n">
+        <v>2</v>
+      </c>
+      <c r="U263" t="n">
+        <v>3</v>
+      </c>
+      <c r="V263" t="n">
+        <v>0</v>
+      </c>
+      <c r="W263" t="n">
+        <v>1</v>
+      </c>
+      <c r="X263" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y263" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z263" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA263" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="n">
+        <v>1631169</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>Josh Minott</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>3:21</t>
+        </is>
+      </c>
+      <c r="I264" t="n">
+        <v>1</v>
+      </c>
+      <c r="J264" t="n">
+        <v>2</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L264" t="n">
+        <v>0</v>
+      </c>
+      <c r="M264" t="n">
+        <v>1</v>
+      </c>
+      <c r="N264" t="n">
+        <v>0</v>
+      </c>
+      <c r="O264" t="n">
+        <v>0</v>
+      </c>
+      <c r="P264" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q264" t="n">
+        <v>0</v>
+      </c>
+      <c r="R264" t="n">
+        <v>0</v>
+      </c>
+      <c r="S264" t="n">
+        <v>0</v>
+      </c>
+      <c r="T264" t="n">
+        <v>0</v>
+      </c>
+      <c r="U264" t="n">
+        <v>1</v>
+      </c>
+      <c r="V264" t="n">
+        <v>0</v>
+      </c>
+      <c r="W264" t="n">
+        <v>0</v>
+      </c>
+      <c r="X264" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y264" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z264" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA264" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="n">
+        <v>1630545</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Terrence Shannon Jr.</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>3:21</t>
+        </is>
+      </c>
+      <c r="I265" t="n">
+        <v>1</v>
+      </c>
+      <c r="J265" t="n">
+        <v>2</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L265" t="n">
+        <v>0</v>
+      </c>
+      <c r="M265" t="n">
+        <v>0</v>
+      </c>
+      <c r="N265" t="n">
+        <v>0</v>
+      </c>
+      <c r="O265" t="n">
+        <v>0</v>
+      </c>
+      <c r="P265" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q265" t="n">
+        <v>0</v>
+      </c>
+      <c r="R265" t="n">
+        <v>0</v>
+      </c>
+      <c r="S265" t="n">
+        <v>0</v>
+      </c>
+      <c r="T265" t="n">
+        <v>0</v>
+      </c>
+      <c r="U265" t="n">
+        <v>1</v>
+      </c>
+      <c r="V265" t="n">
+        <v>2</v>
+      </c>
+      <c r="W265" t="n">
+        <v>0</v>
+      </c>
+      <c r="X265" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y265" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z265" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA265" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="n">
+        <v>1641740</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Jaylen Clark</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>3:21</t>
+        </is>
+      </c>
+      <c r="I266" t="n">
+        <v>0</v>
+      </c>
+      <c r="J266" t="n">
+        <v>0</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0</v>
+      </c>
+      <c r="L266" t="n">
+        <v>0</v>
+      </c>
+      <c r="M266" t="n">
+        <v>0</v>
+      </c>
+      <c r="N266" t="n">
+        <v>0</v>
+      </c>
+      <c r="O266" t="n">
+        <v>0</v>
+      </c>
+      <c r="P266" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q266" t="n">
+        <v>0</v>
+      </c>
+      <c r="R266" t="n">
+        <v>0</v>
+      </c>
+      <c r="S266" t="n">
+        <v>1</v>
+      </c>
+      <c r="T266" t="n">
+        <v>1</v>
+      </c>
+      <c r="U266" t="n">
+        <v>0</v>
+      </c>
+      <c r="V266" t="n">
+        <v>0</v>
+      </c>
+      <c r="W266" t="n">
+        <v>0</v>
+      </c>
+      <c r="X266" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y266" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z266" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA266" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="n">
+        <v>1631159</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Leonard Miller</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>3:10</t>
+        </is>
+      </c>
+      <c r="I267" t="n">
+        <v>1</v>
+      </c>
+      <c r="J267" t="n">
+        <v>2</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L267" t="n">
+        <v>0</v>
+      </c>
+      <c r="M267" t="n">
+        <v>0</v>
+      </c>
+      <c r="N267" t="n">
+        <v>0</v>
+      </c>
+      <c r="O267" t="n">
+        <v>0</v>
+      </c>
+      <c r="P267" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q267" t="n">
+        <v>0</v>
+      </c>
+      <c r="R267" t="n">
+        <v>1</v>
+      </c>
+      <c r="S267" t="n">
+        <v>0</v>
+      </c>
+      <c r="T267" t="n">
+        <v>1</v>
+      </c>
+      <c r="U267" t="n">
+        <v>0</v>
+      </c>
+      <c r="V267" t="n">
+        <v>0</v>
+      </c>
+      <c r="W267" t="n">
+        <v>0</v>
+      </c>
+      <c r="X267" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y267" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z267" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA267" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="n">
+        <v>1630568</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Luka Garza</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>2:02</t>
+        </is>
+      </c>
+      <c r="I268" t="n">
+        <v>0</v>
+      </c>
+      <c r="J268" t="n">
+        <v>0</v>
+      </c>
+      <c r="K268" t="n">
+        <v>0</v>
+      </c>
+      <c r="L268" t="n">
+        <v>0</v>
+      </c>
+      <c r="M268" t="n">
+        <v>0</v>
+      </c>
+      <c r="N268" t="n">
+        <v>0</v>
+      </c>
+      <c r="O268" t="n">
+        <v>0</v>
+      </c>
+      <c r="P268" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q268" t="n">
+        <v>0</v>
+      </c>
+      <c r="R268" t="n">
+        <v>0</v>
+      </c>
+      <c r="S268" t="n">
+        <v>0</v>
+      </c>
+      <c r="T268" t="n">
+        <v>0</v>
+      </c>
+      <c r="U268" t="n">
+        <v>0</v>
+      </c>
+      <c r="V268" t="n">
+        <v>0</v>
+      </c>
+      <c r="W268" t="n">
+        <v>0</v>
+      </c>
+      <c r="X268" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y268" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z268" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA268" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="n">
+        <v>204060</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Joe Ingles</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr"/>
+      <c r="I269" t="n">
+        <v>0</v>
+      </c>
+      <c r="J269" t="n">
+        <v>0</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0</v>
+      </c>
+      <c r="L269" t="n">
+        <v>0</v>
+      </c>
+      <c r="M269" t="n">
+        <v>0</v>
+      </c>
+      <c r="N269" t="n">
+        <v>0</v>
+      </c>
+      <c r="O269" t="n">
+        <v>0</v>
+      </c>
+      <c r="P269" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q269" t="n">
+        <v>0</v>
+      </c>
+      <c r="R269" t="n">
+        <v>0</v>
+      </c>
+      <c r="S269" t="n">
+        <v>0</v>
+      </c>
+      <c r="T269" t="n">
+        <v>0</v>
+      </c>
+      <c r="U269" t="n">
+        <v>0</v>
+      </c>
+      <c r="V269" t="n">
+        <v>0</v>
+      </c>
+      <c r="W269" t="n">
+        <v>0</v>
+      </c>
+      <c r="X269" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y269" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z269" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA269" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add GSW vs MIN GM3 stats & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA269"/>
+  <dimension ref="A1:AA299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25773,6 +25773,2808 @@
         <v>0</v>
       </c>
     </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>1630183</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Jaden McDaniels</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>42:11</t>
+        </is>
+      </c>
+      <c r="I270" t="n">
+        <v>4</v>
+      </c>
+      <c r="J270" t="n">
+        <v>7</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="L270" t="n">
+        <v>3</v>
+      </c>
+      <c r="M270" t="n">
+        <v>4</v>
+      </c>
+      <c r="N270" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O270" t="n">
+        <v>4</v>
+      </c>
+      <c r="P270" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q270" t="n">
+        <v>1</v>
+      </c>
+      <c r="R270" t="n">
+        <v>0</v>
+      </c>
+      <c r="S270" t="n">
+        <v>6</v>
+      </c>
+      <c r="T270" t="n">
+        <v>6</v>
+      </c>
+      <c r="U270" t="n">
+        <v>1</v>
+      </c>
+      <c r="V270" t="n">
+        <v>1</v>
+      </c>
+      <c r="W270" t="n">
+        <v>2</v>
+      </c>
+      <c r="X270" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y270" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z270" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA270" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="n">
+        <v>203944</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Julius Randle</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>40:26</t>
+        </is>
+      </c>
+      <c r="I271" t="n">
+        <v>10</v>
+      </c>
+      <c r="J271" t="n">
+        <v>23</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0.435</v>
+      </c>
+      <c r="L271" t="n">
+        <v>1</v>
+      </c>
+      <c r="M271" t="n">
+        <v>6</v>
+      </c>
+      <c r="N271" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="O271" t="n">
+        <v>3</v>
+      </c>
+      <c r="P271" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q271" t="n">
+        <v>1</v>
+      </c>
+      <c r="R271" t="n">
+        <v>3</v>
+      </c>
+      <c r="S271" t="n">
+        <v>7</v>
+      </c>
+      <c r="T271" t="n">
+        <v>10</v>
+      </c>
+      <c r="U271" t="n">
+        <v>12</v>
+      </c>
+      <c r="V271" t="n">
+        <v>3</v>
+      </c>
+      <c r="W271" t="n">
+        <v>0</v>
+      </c>
+      <c r="X271" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y271" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z271" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA271" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>203497</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Rudy Gobert</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>26:45</t>
+        </is>
+      </c>
+      <c r="I272" t="n">
+        <v>2</v>
+      </c>
+      <c r="J272" t="n">
+        <v>4</v>
+      </c>
+      <c r="K272" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L272" t="n">
+        <v>0</v>
+      </c>
+      <c r="M272" t="n">
+        <v>0</v>
+      </c>
+      <c r="N272" t="n">
+        <v>0</v>
+      </c>
+      <c r="O272" t="n">
+        <v>5</v>
+      </c>
+      <c r="P272" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q272" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="R272" t="n">
+        <v>4</v>
+      </c>
+      <c r="S272" t="n">
+        <v>9</v>
+      </c>
+      <c r="T272" t="n">
+        <v>13</v>
+      </c>
+      <c r="U272" t="n">
+        <v>0</v>
+      </c>
+      <c r="V272" t="n">
+        <v>0</v>
+      </c>
+      <c r="W272" t="n">
+        <v>4</v>
+      </c>
+      <c r="X272" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y272" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z272" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA272" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="n">
+        <v>1630162</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Anthony Edwards</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>43:49</t>
+        </is>
+      </c>
+      <c r="I273" t="n">
+        <v>13</v>
+      </c>
+      <c r="J273" t="n">
+        <v>28</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0.464</v>
+      </c>
+      <c r="L273" t="n">
+        <v>5</v>
+      </c>
+      <c r="M273" t="n">
+        <v>14</v>
+      </c>
+      <c r="N273" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="O273" t="n">
+        <v>5</v>
+      </c>
+      <c r="P273" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q273" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="R273" t="n">
+        <v>1</v>
+      </c>
+      <c r="S273" t="n">
+        <v>3</v>
+      </c>
+      <c r="T273" t="n">
+        <v>4</v>
+      </c>
+      <c r="U273" t="n">
+        <v>4</v>
+      </c>
+      <c r="V273" t="n">
+        <v>0</v>
+      </c>
+      <c r="W273" t="n">
+        <v>1</v>
+      </c>
+      <c r="X273" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y273" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z273" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA273" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="n">
+        <v>201144</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Mike Conley</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>28:18</t>
+        </is>
+      </c>
+      <c r="I274" t="n">
+        <v>3</v>
+      </c>
+      <c r="J274" t="n">
+        <v>9</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L274" t="n">
+        <v>1</v>
+      </c>
+      <c r="M274" t="n">
+        <v>4</v>
+      </c>
+      <c r="N274" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O274" t="n">
+        <v>0</v>
+      </c>
+      <c r="P274" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q274" t="n">
+        <v>0</v>
+      </c>
+      <c r="R274" t="n">
+        <v>3</v>
+      </c>
+      <c r="S274" t="n">
+        <v>1</v>
+      </c>
+      <c r="T274" t="n">
+        <v>4</v>
+      </c>
+      <c r="U274" t="n">
+        <v>5</v>
+      </c>
+      <c r="V274" t="n">
+        <v>0</v>
+      </c>
+      <c r="W274" t="n">
+        <v>0</v>
+      </c>
+      <c r="X274" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y274" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z274" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA274" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="n">
+        <v>1629675</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Naz Reid</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>24:30</t>
+        </is>
+      </c>
+      <c r="I275" t="n">
+        <v>3</v>
+      </c>
+      <c r="J275" t="n">
+        <v>4</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L275" t="n">
+        <v>3</v>
+      </c>
+      <c r="M275" t="n">
+        <v>3</v>
+      </c>
+      <c r="N275" t="n">
+        <v>1</v>
+      </c>
+      <c r="O275" t="n">
+        <v>0</v>
+      </c>
+      <c r="P275" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q275" t="n">
+        <v>0</v>
+      </c>
+      <c r="R275" t="n">
+        <v>0</v>
+      </c>
+      <c r="S275" t="n">
+        <v>3</v>
+      </c>
+      <c r="T275" t="n">
+        <v>3</v>
+      </c>
+      <c r="U275" t="n">
+        <v>2</v>
+      </c>
+      <c r="V275" t="n">
+        <v>0</v>
+      </c>
+      <c r="W275" t="n">
+        <v>0</v>
+      </c>
+      <c r="X275" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y275" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z275" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA275" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="n">
+        <v>1628978</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Donte DiVincenzo</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>15:49</t>
+        </is>
+      </c>
+      <c r="I276" t="n">
+        <v>1</v>
+      </c>
+      <c r="J276" t="n">
+        <v>3</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L276" t="n">
+        <v>0</v>
+      </c>
+      <c r="M276" t="n">
+        <v>2</v>
+      </c>
+      <c r="N276" t="n">
+        <v>0</v>
+      </c>
+      <c r="O276" t="n">
+        <v>0</v>
+      </c>
+      <c r="P276" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q276" t="n">
+        <v>0</v>
+      </c>
+      <c r="R276" t="n">
+        <v>1</v>
+      </c>
+      <c r="S276" t="n">
+        <v>1</v>
+      </c>
+      <c r="T276" t="n">
+        <v>2</v>
+      </c>
+      <c r="U276" t="n">
+        <v>0</v>
+      </c>
+      <c r="V276" t="n">
+        <v>0</v>
+      </c>
+      <c r="W276" t="n">
+        <v>0</v>
+      </c>
+      <c r="X276" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y276" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z276" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA276" t="n">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="n">
+        <v>1629638</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>18:12</t>
+        </is>
+      </c>
+      <c r="I277" t="n">
+        <v>0</v>
+      </c>
+      <c r="J277" t="n">
+        <v>4</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0</v>
+      </c>
+      <c r="L277" t="n">
+        <v>0</v>
+      </c>
+      <c r="M277" t="n">
+        <v>1</v>
+      </c>
+      <c r="N277" t="n">
+        <v>0</v>
+      </c>
+      <c r="O277" t="n">
+        <v>0</v>
+      </c>
+      <c r="P277" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q277" t="n">
+        <v>0</v>
+      </c>
+      <c r="R277" t="n">
+        <v>1</v>
+      </c>
+      <c r="S277" t="n">
+        <v>1</v>
+      </c>
+      <c r="T277" t="n">
+        <v>2</v>
+      </c>
+      <c r="U277" t="n">
+        <v>4</v>
+      </c>
+      <c r="V277" t="n">
+        <v>0</v>
+      </c>
+      <c r="W277" t="n">
+        <v>0</v>
+      </c>
+      <c r="X277" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y277" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z277" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="n">
+        <v>1641740</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Jaylen Clark</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr"/>
+      <c r="I278" t="n">
+        <v>0</v>
+      </c>
+      <c r="J278" t="n">
+        <v>0</v>
+      </c>
+      <c r="K278" t="n">
+        <v>0</v>
+      </c>
+      <c r="L278" t="n">
+        <v>0</v>
+      </c>
+      <c r="M278" t="n">
+        <v>0</v>
+      </c>
+      <c r="N278" t="n">
+        <v>0</v>
+      </c>
+      <c r="O278" t="n">
+        <v>0</v>
+      </c>
+      <c r="P278" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q278" t="n">
+        <v>0</v>
+      </c>
+      <c r="R278" t="n">
+        <v>0</v>
+      </c>
+      <c r="S278" t="n">
+        <v>0</v>
+      </c>
+      <c r="T278" t="n">
+        <v>0</v>
+      </c>
+      <c r="U278" t="n">
+        <v>0</v>
+      </c>
+      <c r="V278" t="n">
+        <v>0</v>
+      </c>
+      <c r="W278" t="n">
+        <v>0</v>
+      </c>
+      <c r="X278" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y278" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z278" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA278" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="n">
+        <v>1642265</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Rob Dillingham</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr"/>
+      <c r="I279" t="n">
+        <v>0</v>
+      </c>
+      <c r="J279" t="n">
+        <v>0</v>
+      </c>
+      <c r="K279" t="n">
+        <v>0</v>
+      </c>
+      <c r="L279" t="n">
+        <v>0</v>
+      </c>
+      <c r="M279" t="n">
+        <v>0</v>
+      </c>
+      <c r="N279" t="n">
+        <v>0</v>
+      </c>
+      <c r="O279" t="n">
+        <v>0</v>
+      </c>
+      <c r="P279" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q279" t="n">
+        <v>0</v>
+      </c>
+      <c r="R279" t="n">
+        <v>0</v>
+      </c>
+      <c r="S279" t="n">
+        <v>0</v>
+      </c>
+      <c r="T279" t="n">
+        <v>0</v>
+      </c>
+      <c r="U279" t="n">
+        <v>0</v>
+      </c>
+      <c r="V279" t="n">
+        <v>0</v>
+      </c>
+      <c r="W279" t="n">
+        <v>0</v>
+      </c>
+      <c r="X279" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y279" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z279" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA279" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="n">
+        <v>1630568</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Luka Garza</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr"/>
+      <c r="I280" t="n">
+        <v>0</v>
+      </c>
+      <c r="J280" t="n">
+        <v>0</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0</v>
+      </c>
+      <c r="L280" t="n">
+        <v>0</v>
+      </c>
+      <c r="M280" t="n">
+        <v>0</v>
+      </c>
+      <c r="N280" t="n">
+        <v>0</v>
+      </c>
+      <c r="O280" t="n">
+        <v>0</v>
+      </c>
+      <c r="P280" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q280" t="n">
+        <v>0</v>
+      </c>
+      <c r="R280" t="n">
+        <v>0</v>
+      </c>
+      <c r="S280" t="n">
+        <v>0</v>
+      </c>
+      <c r="T280" t="n">
+        <v>0</v>
+      </c>
+      <c r="U280" t="n">
+        <v>0</v>
+      </c>
+      <c r="V280" t="n">
+        <v>0</v>
+      </c>
+      <c r="W280" t="n">
+        <v>0</v>
+      </c>
+      <c r="X280" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y280" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z280" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA280" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="n">
+        <v>204060</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Joe Ingles</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr"/>
+      <c r="I281" t="n">
+        <v>0</v>
+      </c>
+      <c r="J281" t="n">
+        <v>0</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0</v>
+      </c>
+      <c r="L281" t="n">
+        <v>0</v>
+      </c>
+      <c r="M281" t="n">
+        <v>0</v>
+      </c>
+      <c r="N281" t="n">
+        <v>0</v>
+      </c>
+      <c r="O281" t="n">
+        <v>0</v>
+      </c>
+      <c r="P281" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q281" t="n">
+        <v>0</v>
+      </c>
+      <c r="R281" t="n">
+        <v>0</v>
+      </c>
+      <c r="S281" t="n">
+        <v>0</v>
+      </c>
+      <c r="T281" t="n">
+        <v>0</v>
+      </c>
+      <c r="U281" t="n">
+        <v>0</v>
+      </c>
+      <c r="V281" t="n">
+        <v>0</v>
+      </c>
+      <c r="W281" t="n">
+        <v>0</v>
+      </c>
+      <c r="X281" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y281" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z281" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA281" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="n">
+        <v>1631159</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Leonard Miller</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr"/>
+      <c r="I282" t="n">
+        <v>0</v>
+      </c>
+      <c r="J282" t="n">
+        <v>0</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0</v>
+      </c>
+      <c r="L282" t="n">
+        <v>0</v>
+      </c>
+      <c r="M282" t="n">
+        <v>0</v>
+      </c>
+      <c r="N282" t="n">
+        <v>0</v>
+      </c>
+      <c r="O282" t="n">
+        <v>0</v>
+      </c>
+      <c r="P282" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q282" t="n">
+        <v>0</v>
+      </c>
+      <c r="R282" t="n">
+        <v>0</v>
+      </c>
+      <c r="S282" t="n">
+        <v>0</v>
+      </c>
+      <c r="T282" t="n">
+        <v>0</v>
+      </c>
+      <c r="U282" t="n">
+        <v>0</v>
+      </c>
+      <c r="V282" t="n">
+        <v>0</v>
+      </c>
+      <c r="W282" t="n">
+        <v>0</v>
+      </c>
+      <c r="X282" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y282" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z282" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA282" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="n">
+        <v>1631169</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Josh Minott</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr"/>
+      <c r="I283" t="n">
+        <v>0</v>
+      </c>
+      <c r="J283" t="n">
+        <v>0</v>
+      </c>
+      <c r="K283" t="n">
+        <v>0</v>
+      </c>
+      <c r="L283" t="n">
+        <v>0</v>
+      </c>
+      <c r="M283" t="n">
+        <v>0</v>
+      </c>
+      <c r="N283" t="n">
+        <v>0</v>
+      </c>
+      <c r="O283" t="n">
+        <v>0</v>
+      </c>
+      <c r="P283" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q283" t="n">
+        <v>0</v>
+      </c>
+      <c r="R283" t="n">
+        <v>0</v>
+      </c>
+      <c r="S283" t="n">
+        <v>0</v>
+      </c>
+      <c r="T283" t="n">
+        <v>0</v>
+      </c>
+      <c r="U283" t="n">
+        <v>0</v>
+      </c>
+      <c r="V283" t="n">
+        <v>0</v>
+      </c>
+      <c r="W283" t="n">
+        <v>0</v>
+      </c>
+      <c r="X283" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y283" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z283" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA283" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="n">
+        <v>1630545</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Terrence Shannon Jr.</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr"/>
+      <c r="I284" t="n">
+        <v>0</v>
+      </c>
+      <c r="J284" t="n">
+        <v>0</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0</v>
+      </c>
+      <c r="L284" t="n">
+        <v>0</v>
+      </c>
+      <c r="M284" t="n">
+        <v>0</v>
+      </c>
+      <c r="N284" t="n">
+        <v>0</v>
+      </c>
+      <c r="O284" t="n">
+        <v>0</v>
+      </c>
+      <c r="P284" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q284" t="n">
+        <v>0</v>
+      </c>
+      <c r="R284" t="n">
+        <v>0</v>
+      </c>
+      <c r="S284" t="n">
+        <v>0</v>
+      </c>
+      <c r="T284" t="n">
+        <v>0</v>
+      </c>
+      <c r="U284" t="n">
+        <v>0</v>
+      </c>
+      <c r="V284" t="n">
+        <v>0</v>
+      </c>
+      <c r="W284" t="n">
+        <v>0</v>
+      </c>
+      <c r="X284" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y284" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z284" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA284" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>42:59</t>
+        </is>
+      </c>
+      <c r="I285" t="n">
+        <v>12</v>
+      </c>
+      <c r="J285" t="n">
+        <v>26</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="L285" t="n">
+        <v>2</v>
+      </c>
+      <c r="M285" t="n">
+        <v>4</v>
+      </c>
+      <c r="N285" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O285" t="n">
+        <v>7</v>
+      </c>
+      <c r="P285" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q285" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="R285" t="n">
+        <v>1</v>
+      </c>
+      <c r="S285" t="n">
+        <v>6</v>
+      </c>
+      <c r="T285" t="n">
+        <v>7</v>
+      </c>
+      <c r="U285" t="n">
+        <v>7</v>
+      </c>
+      <c r="V285" t="n">
+        <v>0</v>
+      </c>
+      <c r="W285" t="n">
+        <v>0</v>
+      </c>
+      <c r="X285" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y285" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z285" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA285" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>29:08</t>
+        </is>
+      </c>
+      <c r="I286" t="n">
+        <v>1</v>
+      </c>
+      <c r="J286" t="n">
+        <v>4</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L286" t="n">
+        <v>0</v>
+      </c>
+      <c r="M286" t="n">
+        <v>1</v>
+      </c>
+      <c r="N286" t="n">
+        <v>0</v>
+      </c>
+      <c r="O286" t="n">
+        <v>0</v>
+      </c>
+      <c r="P286" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q286" t="n">
+        <v>0</v>
+      </c>
+      <c r="R286" t="n">
+        <v>0</v>
+      </c>
+      <c r="S286" t="n">
+        <v>2</v>
+      </c>
+      <c r="T286" t="n">
+        <v>2</v>
+      </c>
+      <c r="U286" t="n">
+        <v>4</v>
+      </c>
+      <c r="V286" t="n">
+        <v>2</v>
+      </c>
+      <c r="W286" t="n">
+        <v>0</v>
+      </c>
+      <c r="X286" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y286" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z286" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA286" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="I287" t="n">
+        <v>3</v>
+      </c>
+      <c r="J287" t="n">
+        <v>4</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L287" t="n">
+        <v>0</v>
+      </c>
+      <c r="M287" t="n">
+        <v>0</v>
+      </c>
+      <c r="N287" t="n">
+        <v>0</v>
+      </c>
+      <c r="O287" t="n">
+        <v>1</v>
+      </c>
+      <c r="P287" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q287" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R287" t="n">
+        <v>1</v>
+      </c>
+      <c r="S287" t="n">
+        <v>1</v>
+      </c>
+      <c r="T287" t="n">
+        <v>2</v>
+      </c>
+      <c r="U287" t="n">
+        <v>0</v>
+      </c>
+      <c r="V287" t="n">
+        <v>0</v>
+      </c>
+      <c r="W287" t="n">
+        <v>1</v>
+      </c>
+      <c r="X287" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y287" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z287" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA287" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>32:21</t>
+        </is>
+      </c>
+      <c r="I288" t="n">
+        <v>5</v>
+      </c>
+      <c r="J288" t="n">
+        <v>11</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="L288" t="n">
+        <v>4</v>
+      </c>
+      <c r="M288" t="n">
+        <v>8</v>
+      </c>
+      <c r="N288" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O288" t="n">
+        <v>0</v>
+      </c>
+      <c r="P288" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q288" t="n">
+        <v>0</v>
+      </c>
+      <c r="R288" t="n">
+        <v>2</v>
+      </c>
+      <c r="S288" t="n">
+        <v>2</v>
+      </c>
+      <c r="T288" t="n">
+        <v>4</v>
+      </c>
+      <c r="U288" t="n">
+        <v>5</v>
+      </c>
+      <c r="V288" t="n">
+        <v>0</v>
+      </c>
+      <c r="W288" t="n">
+        <v>2</v>
+      </c>
+      <c r="X288" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y288" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z288" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA288" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>39:08</t>
+        </is>
+      </c>
+      <c r="I289" t="n">
+        <v>1</v>
+      </c>
+      <c r="J289" t="n">
+        <v>10</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L289" t="n">
+        <v>1</v>
+      </c>
+      <c r="M289" t="n">
+        <v>4</v>
+      </c>
+      <c r="N289" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O289" t="n">
+        <v>2</v>
+      </c>
+      <c r="P289" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q289" t="n">
+        <v>1</v>
+      </c>
+      <c r="R289" t="n">
+        <v>3</v>
+      </c>
+      <c r="S289" t="n">
+        <v>5</v>
+      </c>
+      <c r="T289" t="n">
+        <v>8</v>
+      </c>
+      <c r="U289" t="n">
+        <v>2</v>
+      </c>
+      <c r="V289" t="n">
+        <v>1</v>
+      </c>
+      <c r="W289" t="n">
+        <v>0</v>
+      </c>
+      <c r="X289" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y289" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z289" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA289" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>2:31</t>
+        </is>
+      </c>
+      <c r="I290" t="n">
+        <v>0</v>
+      </c>
+      <c r="J290" t="n">
+        <v>0</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0</v>
+      </c>
+      <c r="L290" t="n">
+        <v>0</v>
+      </c>
+      <c r="M290" t="n">
+        <v>0</v>
+      </c>
+      <c r="N290" t="n">
+        <v>0</v>
+      </c>
+      <c r="O290" t="n">
+        <v>0</v>
+      </c>
+      <c r="P290" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q290" t="n">
+        <v>0</v>
+      </c>
+      <c r="R290" t="n">
+        <v>0</v>
+      </c>
+      <c r="S290" t="n">
+        <v>0</v>
+      </c>
+      <c r="T290" t="n">
+        <v>0</v>
+      </c>
+      <c r="U290" t="n">
+        <v>0</v>
+      </c>
+      <c r="V290" t="n">
+        <v>0</v>
+      </c>
+      <c r="W290" t="n">
+        <v>0</v>
+      </c>
+      <c r="X290" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y290" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z290" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA290" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>25:33</t>
+        </is>
+      </c>
+      <c r="I291" t="n">
+        <v>1</v>
+      </c>
+      <c r="J291" t="n">
+        <v>4</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L291" t="n">
+        <v>0</v>
+      </c>
+      <c r="M291" t="n">
+        <v>2</v>
+      </c>
+      <c r="N291" t="n">
+        <v>0</v>
+      </c>
+      <c r="O291" t="n">
+        <v>0</v>
+      </c>
+      <c r="P291" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q291" t="n">
+        <v>0</v>
+      </c>
+      <c r="R291" t="n">
+        <v>0</v>
+      </c>
+      <c r="S291" t="n">
+        <v>1</v>
+      </c>
+      <c r="T291" t="n">
+        <v>1</v>
+      </c>
+      <c r="U291" t="n">
+        <v>0</v>
+      </c>
+      <c r="V291" t="n">
+        <v>1</v>
+      </c>
+      <c r="W291" t="n">
+        <v>0</v>
+      </c>
+      <c r="X291" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y291" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z291" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA291" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>35:52</t>
+        </is>
+      </c>
+      <c r="I292" t="n">
+        <v>11</v>
+      </c>
+      <c r="J292" t="n">
+        <v>18</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0.611</v>
+      </c>
+      <c r="L292" t="n">
+        <v>3</v>
+      </c>
+      <c r="M292" t="n">
+        <v>4</v>
+      </c>
+      <c r="N292" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O292" t="n">
+        <v>5</v>
+      </c>
+      <c r="P292" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q292" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="R292" t="n">
+        <v>1</v>
+      </c>
+      <c r="S292" t="n">
+        <v>5</v>
+      </c>
+      <c r="T292" t="n">
+        <v>6</v>
+      </c>
+      <c r="U292" t="n">
+        <v>3</v>
+      </c>
+      <c r="V292" t="n">
+        <v>0</v>
+      </c>
+      <c r="W292" t="n">
+        <v>2</v>
+      </c>
+      <c r="X292" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y292" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z292" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA292" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="I293" t="n">
+        <v>1</v>
+      </c>
+      <c r="J293" t="n">
+        <v>4</v>
+      </c>
+      <c r="K293" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L293" t="n">
+        <v>0</v>
+      </c>
+      <c r="M293" t="n">
+        <v>0</v>
+      </c>
+      <c r="N293" t="n">
+        <v>0</v>
+      </c>
+      <c r="O293" t="n">
+        <v>2</v>
+      </c>
+      <c r="P293" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q293" t="n">
+        <v>1</v>
+      </c>
+      <c r="R293" t="n">
+        <v>4</v>
+      </c>
+      <c r="S293" t="n">
+        <v>2</v>
+      </c>
+      <c r="T293" t="n">
+        <v>6</v>
+      </c>
+      <c r="U293" t="n">
+        <v>0</v>
+      </c>
+      <c r="V293" t="n">
+        <v>2</v>
+      </c>
+      <c r="W293" t="n">
+        <v>2</v>
+      </c>
+      <c r="X293" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y293" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z293" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA293" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>3:20</t>
+        </is>
+      </c>
+      <c r="I294" t="n">
+        <v>0</v>
+      </c>
+      <c r="J294" t="n">
+        <v>0</v>
+      </c>
+      <c r="K294" t="n">
+        <v>0</v>
+      </c>
+      <c r="L294" t="n">
+        <v>0</v>
+      </c>
+      <c r="M294" t="n">
+        <v>0</v>
+      </c>
+      <c r="N294" t="n">
+        <v>0</v>
+      </c>
+      <c r="O294" t="n">
+        <v>0</v>
+      </c>
+      <c r="P294" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q294" t="n">
+        <v>0</v>
+      </c>
+      <c r="R294" t="n">
+        <v>0</v>
+      </c>
+      <c r="S294" t="n">
+        <v>0</v>
+      </c>
+      <c r="T294" t="n">
+        <v>0</v>
+      </c>
+      <c r="U294" t="n">
+        <v>0</v>
+      </c>
+      <c r="V294" t="n">
+        <v>0</v>
+      </c>
+      <c r="W294" t="n">
+        <v>0</v>
+      </c>
+      <c r="X294" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y294" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z294" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA294" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr"/>
+      <c r="I295" t="n">
+        <v>0</v>
+      </c>
+      <c r="J295" t="n">
+        <v>0</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0</v>
+      </c>
+      <c r="L295" t="n">
+        <v>0</v>
+      </c>
+      <c r="M295" t="n">
+        <v>0</v>
+      </c>
+      <c r="N295" t="n">
+        <v>0</v>
+      </c>
+      <c r="O295" t="n">
+        <v>0</v>
+      </c>
+      <c r="P295" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q295" t="n">
+        <v>0</v>
+      </c>
+      <c r="R295" t="n">
+        <v>0</v>
+      </c>
+      <c r="S295" t="n">
+        <v>0</v>
+      </c>
+      <c r="T295" t="n">
+        <v>0</v>
+      </c>
+      <c r="U295" t="n">
+        <v>0</v>
+      </c>
+      <c r="V295" t="n">
+        <v>0</v>
+      </c>
+      <c r="W295" t="n">
+        <v>0</v>
+      </c>
+      <c r="X295" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y295" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA295" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr"/>
+      <c r="I296" t="n">
+        <v>0</v>
+      </c>
+      <c r="J296" t="n">
+        <v>0</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0</v>
+      </c>
+      <c r="L296" t="n">
+        <v>0</v>
+      </c>
+      <c r="M296" t="n">
+        <v>0</v>
+      </c>
+      <c r="N296" t="n">
+        <v>0</v>
+      </c>
+      <c r="O296" t="n">
+        <v>0</v>
+      </c>
+      <c r="P296" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q296" t="n">
+        <v>0</v>
+      </c>
+      <c r="R296" t="n">
+        <v>0</v>
+      </c>
+      <c r="S296" t="n">
+        <v>0</v>
+      </c>
+      <c r="T296" t="n">
+        <v>0</v>
+      </c>
+      <c r="U296" t="n">
+        <v>0</v>
+      </c>
+      <c r="V296" t="n">
+        <v>0</v>
+      </c>
+      <c r="W296" t="n">
+        <v>0</v>
+      </c>
+      <c r="X296" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y296" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA296" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr"/>
+      <c r="I297" t="n">
+        <v>0</v>
+      </c>
+      <c r="J297" t="n">
+        <v>0</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0</v>
+      </c>
+      <c r="L297" t="n">
+        <v>0</v>
+      </c>
+      <c r="M297" t="n">
+        <v>0</v>
+      </c>
+      <c r="N297" t="n">
+        <v>0</v>
+      </c>
+      <c r="O297" t="n">
+        <v>0</v>
+      </c>
+      <c r="P297" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q297" t="n">
+        <v>0</v>
+      </c>
+      <c r="R297" t="n">
+        <v>0</v>
+      </c>
+      <c r="S297" t="n">
+        <v>0</v>
+      </c>
+      <c r="T297" t="n">
+        <v>0</v>
+      </c>
+      <c r="U297" t="n">
+        <v>0</v>
+      </c>
+      <c r="V297" t="n">
+        <v>0</v>
+      </c>
+      <c r="W297" t="n">
+        <v>0</v>
+      </c>
+      <c r="X297" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y297" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA297" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr"/>
+      <c r="I298" t="n">
+        <v>0</v>
+      </c>
+      <c r="J298" t="n">
+        <v>0</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0</v>
+      </c>
+      <c r="L298" t="n">
+        <v>0</v>
+      </c>
+      <c r="M298" t="n">
+        <v>0</v>
+      </c>
+      <c r="N298" t="n">
+        <v>0</v>
+      </c>
+      <c r="O298" t="n">
+        <v>0</v>
+      </c>
+      <c r="P298" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q298" t="n">
+        <v>0</v>
+      </c>
+      <c r="R298" t="n">
+        <v>0</v>
+      </c>
+      <c r="S298" t="n">
+        <v>0</v>
+      </c>
+      <c r="T298" t="n">
+        <v>0</v>
+      </c>
+      <c r="U298" t="n">
+        <v>0</v>
+      </c>
+      <c r="V298" t="n">
+        <v>0</v>
+      </c>
+      <c r="W298" t="n">
+        <v>0</v>
+      </c>
+      <c r="X298" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y298" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z298" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr"/>
+      <c r="I299" t="n">
+        <v>0</v>
+      </c>
+      <c r="J299" t="n">
+        <v>0</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0</v>
+      </c>
+      <c r="L299" t="n">
+        <v>0</v>
+      </c>
+      <c r="M299" t="n">
+        <v>0</v>
+      </c>
+      <c r="N299" t="n">
+        <v>0</v>
+      </c>
+      <c r="O299" t="n">
+        <v>0</v>
+      </c>
+      <c r="P299" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q299" t="n">
+        <v>0</v>
+      </c>
+      <c r="R299" t="n">
+        <v>0</v>
+      </c>
+      <c r="S299" t="n">
+        <v>0</v>
+      </c>
+      <c r="T299" t="n">
+        <v>0</v>
+      </c>
+      <c r="U299" t="n">
+        <v>0</v>
+      </c>
+      <c r="V299" t="n">
+        <v>0</v>
+      </c>
+      <c r="W299" t="n">
+        <v>0</v>
+      </c>
+      <c r="X299" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y299" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA299" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add GSW vs MIN GM4 stats & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA299"/>
+  <dimension ref="A1:AA329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28575,6 +28575,2824 @@
         <v>0</v>
       </c>
     </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="n">
+        <v>1630183</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Jaden McDaniels</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>40:18</t>
+        </is>
+      </c>
+      <c r="I300" t="n">
+        <v>4</v>
+      </c>
+      <c r="J300" t="n">
+        <v>8</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L300" t="n">
+        <v>0</v>
+      </c>
+      <c r="M300" t="n">
+        <v>1</v>
+      </c>
+      <c r="N300" t="n">
+        <v>0</v>
+      </c>
+      <c r="O300" t="n">
+        <v>2</v>
+      </c>
+      <c r="P300" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q300" t="n">
+        <v>1</v>
+      </c>
+      <c r="R300" t="n">
+        <v>1</v>
+      </c>
+      <c r="S300" t="n">
+        <v>12</v>
+      </c>
+      <c r="T300" t="n">
+        <v>13</v>
+      </c>
+      <c r="U300" t="n">
+        <v>2</v>
+      </c>
+      <c r="V300" t="n">
+        <v>1</v>
+      </c>
+      <c r="W300" t="n">
+        <v>1</v>
+      </c>
+      <c r="X300" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y300" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z300" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA300" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="n">
+        <v>203944</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Julius Randle</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>40:49</t>
+        </is>
+      </c>
+      <c r="I301" t="n">
+        <v>11</v>
+      </c>
+      <c r="J301" t="n">
+        <v>21</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="L301" t="n">
+        <v>4</v>
+      </c>
+      <c r="M301" t="n">
+        <v>8</v>
+      </c>
+      <c r="N301" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O301" t="n">
+        <v>5</v>
+      </c>
+      <c r="P301" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q301" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="R301" t="n">
+        <v>0</v>
+      </c>
+      <c r="S301" t="n">
+        <v>5</v>
+      </c>
+      <c r="T301" t="n">
+        <v>5</v>
+      </c>
+      <c r="U301" t="n">
+        <v>3</v>
+      </c>
+      <c r="V301" t="n">
+        <v>1</v>
+      </c>
+      <c r="W301" t="n">
+        <v>1</v>
+      </c>
+      <c r="X301" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y301" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z301" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA301" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="n">
+        <v>203497</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Rudy Gobert</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>29:46</t>
+        </is>
+      </c>
+      <c r="I302" t="n">
+        <v>2</v>
+      </c>
+      <c r="J302" t="n">
+        <v>4</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L302" t="n">
+        <v>0</v>
+      </c>
+      <c r="M302" t="n">
+        <v>0</v>
+      </c>
+      <c r="N302" t="n">
+        <v>0</v>
+      </c>
+      <c r="O302" t="n">
+        <v>4</v>
+      </c>
+      <c r="P302" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q302" t="n">
+        <v>1</v>
+      </c>
+      <c r="R302" t="n">
+        <v>3</v>
+      </c>
+      <c r="S302" t="n">
+        <v>3</v>
+      </c>
+      <c r="T302" t="n">
+        <v>6</v>
+      </c>
+      <c r="U302" t="n">
+        <v>1</v>
+      </c>
+      <c r="V302" t="n">
+        <v>0</v>
+      </c>
+      <c r="W302" t="n">
+        <v>1</v>
+      </c>
+      <c r="X302" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y302" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z302" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA302" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="n">
+        <v>1630162</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Anthony Edwards</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>33:17</t>
+        </is>
+      </c>
+      <c r="I303" t="n">
+        <v>11</v>
+      </c>
+      <c r="J303" t="n">
+        <v>21</v>
+      </c>
+      <c r="K303" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="L303" t="n">
+        <v>6</v>
+      </c>
+      <c r="M303" t="n">
+        <v>11</v>
+      </c>
+      <c r="N303" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="O303" t="n">
+        <v>2</v>
+      </c>
+      <c r="P303" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q303" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="R303" t="n">
+        <v>0</v>
+      </c>
+      <c r="S303" t="n">
+        <v>4</v>
+      </c>
+      <c r="T303" t="n">
+        <v>4</v>
+      </c>
+      <c r="U303" t="n">
+        <v>5</v>
+      </c>
+      <c r="V303" t="n">
+        <v>2</v>
+      </c>
+      <c r="W303" t="n">
+        <v>0</v>
+      </c>
+      <c r="X303" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y303" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z303" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA303" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="n">
+        <v>201144</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Mike Conley</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>29:23</t>
+        </is>
+      </c>
+      <c r="I304" t="n">
+        <v>2</v>
+      </c>
+      <c r="J304" t="n">
+        <v>9</v>
+      </c>
+      <c r="K304" t="n">
+        <v>0.222</v>
+      </c>
+      <c r="L304" t="n">
+        <v>2</v>
+      </c>
+      <c r="M304" t="n">
+        <v>6</v>
+      </c>
+      <c r="N304" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O304" t="n">
+        <v>5</v>
+      </c>
+      <c r="P304" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q304" t="n">
+        <v>1</v>
+      </c>
+      <c r="R304" t="n">
+        <v>2</v>
+      </c>
+      <c r="S304" t="n">
+        <v>1</v>
+      </c>
+      <c r="T304" t="n">
+        <v>3</v>
+      </c>
+      <c r="U304" t="n">
+        <v>5</v>
+      </c>
+      <c r="V304" t="n">
+        <v>0</v>
+      </c>
+      <c r="W304" t="n">
+        <v>0</v>
+      </c>
+      <c r="X304" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y304" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z304" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA304" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="n">
+        <v>1628978</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Donte DiVincenzo</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>25:40</t>
+        </is>
+      </c>
+      <c r="I305" t="n">
+        <v>2</v>
+      </c>
+      <c r="J305" t="n">
+        <v>7</v>
+      </c>
+      <c r="K305" t="n">
+        <v>0.286</v>
+      </c>
+      <c r="L305" t="n">
+        <v>2</v>
+      </c>
+      <c r="M305" t="n">
+        <v>4</v>
+      </c>
+      <c r="N305" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O305" t="n">
+        <v>3</v>
+      </c>
+      <c r="P305" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q305" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R305" t="n">
+        <v>0</v>
+      </c>
+      <c r="S305" t="n">
+        <v>3</v>
+      </c>
+      <c r="T305" t="n">
+        <v>3</v>
+      </c>
+      <c r="U305" t="n">
+        <v>3</v>
+      </c>
+      <c r="V305" t="n">
+        <v>1</v>
+      </c>
+      <c r="W305" t="n">
+        <v>0</v>
+      </c>
+      <c r="X305" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y305" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z305" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA305" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="n">
+        <v>1629675</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Naz Reid</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>23:33</t>
+        </is>
+      </c>
+      <c r="I306" t="n">
+        <v>2</v>
+      </c>
+      <c r="J306" t="n">
+        <v>4</v>
+      </c>
+      <c r="K306" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L306" t="n">
+        <v>1</v>
+      </c>
+      <c r="M306" t="n">
+        <v>3</v>
+      </c>
+      <c r="N306" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O306" t="n">
+        <v>0</v>
+      </c>
+      <c r="P306" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q306" t="n">
+        <v>0</v>
+      </c>
+      <c r="R306" t="n">
+        <v>0</v>
+      </c>
+      <c r="S306" t="n">
+        <v>2</v>
+      </c>
+      <c r="T306" t="n">
+        <v>2</v>
+      </c>
+      <c r="U306" t="n">
+        <v>1</v>
+      </c>
+      <c r="V306" t="n">
+        <v>3</v>
+      </c>
+      <c r="W306" t="n">
+        <v>1</v>
+      </c>
+      <c r="X306" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y306" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z306" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA306" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="n">
+        <v>1629638</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="I307" t="n">
+        <v>5</v>
+      </c>
+      <c r="J307" t="n">
+        <v>5</v>
+      </c>
+      <c r="K307" t="n">
+        <v>1</v>
+      </c>
+      <c r="L307" t="n">
+        <v>1</v>
+      </c>
+      <c r="M307" t="n">
+        <v>1</v>
+      </c>
+      <c r="N307" t="n">
+        <v>1</v>
+      </c>
+      <c r="O307" t="n">
+        <v>2</v>
+      </c>
+      <c r="P307" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q307" t="n">
+        <v>1</v>
+      </c>
+      <c r="R307" t="n">
+        <v>0</v>
+      </c>
+      <c r="S307" t="n">
+        <v>2</v>
+      </c>
+      <c r="T307" t="n">
+        <v>2</v>
+      </c>
+      <c r="U307" t="n">
+        <v>2</v>
+      </c>
+      <c r="V307" t="n">
+        <v>1</v>
+      </c>
+      <c r="W307" t="n">
+        <v>1</v>
+      </c>
+      <c r="X307" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y307" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z307" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA307" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="n">
+        <v>1641740</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Jaylen Clark</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr"/>
+      <c r="I308" t="n">
+        <v>0</v>
+      </c>
+      <c r="J308" t="n">
+        <v>0</v>
+      </c>
+      <c r="K308" t="n">
+        <v>0</v>
+      </c>
+      <c r="L308" t="n">
+        <v>0</v>
+      </c>
+      <c r="M308" t="n">
+        <v>0</v>
+      </c>
+      <c r="N308" t="n">
+        <v>0</v>
+      </c>
+      <c r="O308" t="n">
+        <v>0</v>
+      </c>
+      <c r="P308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q308" t="n">
+        <v>0</v>
+      </c>
+      <c r="R308" t="n">
+        <v>0</v>
+      </c>
+      <c r="S308" t="n">
+        <v>0</v>
+      </c>
+      <c r="T308" t="n">
+        <v>0</v>
+      </c>
+      <c r="U308" t="n">
+        <v>0</v>
+      </c>
+      <c r="V308" t="n">
+        <v>0</v>
+      </c>
+      <c r="W308" t="n">
+        <v>0</v>
+      </c>
+      <c r="X308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y308" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z308" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA308" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="n">
+        <v>1642265</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Rob Dillingham</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr"/>
+      <c r="I309" t="n">
+        <v>0</v>
+      </c>
+      <c r="J309" t="n">
+        <v>0</v>
+      </c>
+      <c r="K309" t="n">
+        <v>0</v>
+      </c>
+      <c r="L309" t="n">
+        <v>0</v>
+      </c>
+      <c r="M309" t="n">
+        <v>0</v>
+      </c>
+      <c r="N309" t="n">
+        <v>0</v>
+      </c>
+      <c r="O309" t="n">
+        <v>0</v>
+      </c>
+      <c r="P309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q309" t="n">
+        <v>0</v>
+      </c>
+      <c r="R309" t="n">
+        <v>0</v>
+      </c>
+      <c r="S309" t="n">
+        <v>0</v>
+      </c>
+      <c r="T309" t="n">
+        <v>0</v>
+      </c>
+      <c r="U309" t="n">
+        <v>0</v>
+      </c>
+      <c r="V309" t="n">
+        <v>0</v>
+      </c>
+      <c r="W309" t="n">
+        <v>0</v>
+      </c>
+      <c r="X309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y309" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA309" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="n">
+        <v>1630568</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Luka Garza</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr"/>
+      <c r="I310" t="n">
+        <v>0</v>
+      </c>
+      <c r="J310" t="n">
+        <v>0</v>
+      </c>
+      <c r="K310" t="n">
+        <v>0</v>
+      </c>
+      <c r="L310" t="n">
+        <v>0</v>
+      </c>
+      <c r="M310" t="n">
+        <v>0</v>
+      </c>
+      <c r="N310" t="n">
+        <v>0</v>
+      </c>
+      <c r="O310" t="n">
+        <v>0</v>
+      </c>
+      <c r="P310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q310" t="n">
+        <v>0</v>
+      </c>
+      <c r="R310" t="n">
+        <v>0</v>
+      </c>
+      <c r="S310" t="n">
+        <v>0</v>
+      </c>
+      <c r="T310" t="n">
+        <v>0</v>
+      </c>
+      <c r="U310" t="n">
+        <v>0</v>
+      </c>
+      <c r="V310" t="n">
+        <v>0</v>
+      </c>
+      <c r="W310" t="n">
+        <v>0</v>
+      </c>
+      <c r="X310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y310" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z310" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA310" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="n">
+        <v>204060</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Joe Ingles</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr"/>
+      <c r="I311" t="n">
+        <v>0</v>
+      </c>
+      <c r="J311" t="n">
+        <v>0</v>
+      </c>
+      <c r="K311" t="n">
+        <v>0</v>
+      </c>
+      <c r="L311" t="n">
+        <v>0</v>
+      </c>
+      <c r="M311" t="n">
+        <v>0</v>
+      </c>
+      <c r="N311" t="n">
+        <v>0</v>
+      </c>
+      <c r="O311" t="n">
+        <v>0</v>
+      </c>
+      <c r="P311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q311" t="n">
+        <v>0</v>
+      </c>
+      <c r="R311" t="n">
+        <v>0</v>
+      </c>
+      <c r="S311" t="n">
+        <v>0</v>
+      </c>
+      <c r="T311" t="n">
+        <v>0</v>
+      </c>
+      <c r="U311" t="n">
+        <v>0</v>
+      </c>
+      <c r="V311" t="n">
+        <v>0</v>
+      </c>
+      <c r="W311" t="n">
+        <v>0</v>
+      </c>
+      <c r="X311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y311" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z311" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA311" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="n">
+        <v>1631159</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Leonard Miller</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr"/>
+      <c r="I312" t="n">
+        <v>0</v>
+      </c>
+      <c r="J312" t="n">
+        <v>0</v>
+      </c>
+      <c r="K312" t="n">
+        <v>0</v>
+      </c>
+      <c r="L312" t="n">
+        <v>0</v>
+      </c>
+      <c r="M312" t="n">
+        <v>0</v>
+      </c>
+      <c r="N312" t="n">
+        <v>0</v>
+      </c>
+      <c r="O312" t="n">
+        <v>0</v>
+      </c>
+      <c r="P312" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q312" t="n">
+        <v>0</v>
+      </c>
+      <c r="R312" t="n">
+        <v>0</v>
+      </c>
+      <c r="S312" t="n">
+        <v>0</v>
+      </c>
+      <c r="T312" t="n">
+        <v>0</v>
+      </c>
+      <c r="U312" t="n">
+        <v>0</v>
+      </c>
+      <c r="V312" t="n">
+        <v>0</v>
+      </c>
+      <c r="W312" t="n">
+        <v>0</v>
+      </c>
+      <c r="X312" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y312" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z312" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA312" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="n">
+        <v>1631169</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Josh Minott</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr"/>
+      <c r="I313" t="n">
+        <v>0</v>
+      </c>
+      <c r="J313" t="n">
+        <v>0</v>
+      </c>
+      <c r="K313" t="n">
+        <v>0</v>
+      </c>
+      <c r="L313" t="n">
+        <v>0</v>
+      </c>
+      <c r="M313" t="n">
+        <v>0</v>
+      </c>
+      <c r="N313" t="n">
+        <v>0</v>
+      </c>
+      <c r="O313" t="n">
+        <v>0</v>
+      </c>
+      <c r="P313" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q313" t="n">
+        <v>0</v>
+      </c>
+      <c r="R313" t="n">
+        <v>0</v>
+      </c>
+      <c r="S313" t="n">
+        <v>0</v>
+      </c>
+      <c r="T313" t="n">
+        <v>0</v>
+      </c>
+      <c r="U313" t="n">
+        <v>0</v>
+      </c>
+      <c r="V313" t="n">
+        <v>0</v>
+      </c>
+      <c r="W313" t="n">
+        <v>0</v>
+      </c>
+      <c r="X313" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y313" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z313" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA313" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="n">
+        <v>1630545</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Terrence Shannon Jr.</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr"/>
+      <c r="I314" t="n">
+        <v>0</v>
+      </c>
+      <c r="J314" t="n">
+        <v>0</v>
+      </c>
+      <c r="K314" t="n">
+        <v>0</v>
+      </c>
+      <c r="L314" t="n">
+        <v>0</v>
+      </c>
+      <c r="M314" t="n">
+        <v>0</v>
+      </c>
+      <c r="N314" t="n">
+        <v>0</v>
+      </c>
+      <c r="O314" t="n">
+        <v>0</v>
+      </c>
+      <c r="P314" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q314" t="n">
+        <v>0</v>
+      </c>
+      <c r="R314" t="n">
+        <v>0</v>
+      </c>
+      <c r="S314" t="n">
+        <v>0</v>
+      </c>
+      <c r="T314" t="n">
+        <v>0</v>
+      </c>
+      <c r="U314" t="n">
+        <v>0</v>
+      </c>
+      <c r="V314" t="n">
+        <v>0</v>
+      </c>
+      <c r="W314" t="n">
+        <v>0</v>
+      </c>
+      <c r="X314" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y314" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z314" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA314" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>34:21</t>
+        </is>
+      </c>
+      <c r="I315" t="n">
+        <v>5</v>
+      </c>
+      <c r="J315" t="n">
+        <v>9</v>
+      </c>
+      <c r="K315" t="n">
+        <v>0.556</v>
+      </c>
+      <c r="L315" t="n">
+        <v>0</v>
+      </c>
+      <c r="M315" t="n">
+        <v>1</v>
+      </c>
+      <c r="N315" t="n">
+        <v>0</v>
+      </c>
+      <c r="O315" t="n">
+        <v>4</v>
+      </c>
+      <c r="P315" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q315" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R315" t="n">
+        <v>3</v>
+      </c>
+      <c r="S315" t="n">
+        <v>3</v>
+      </c>
+      <c r="T315" t="n">
+        <v>6</v>
+      </c>
+      <c r="U315" t="n">
+        <v>3</v>
+      </c>
+      <c r="V315" t="n">
+        <v>0</v>
+      </c>
+      <c r="W315" t="n">
+        <v>1</v>
+      </c>
+      <c r="X315" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y315" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z315" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA315" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>33:53</t>
+        </is>
+      </c>
+      <c r="I316" t="n">
+        <v>6</v>
+      </c>
+      <c r="J316" t="n">
+        <v>14</v>
+      </c>
+      <c r="K316" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="L316" t="n">
+        <v>2</v>
+      </c>
+      <c r="M316" t="n">
+        <v>6</v>
+      </c>
+      <c r="N316" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O316" t="n">
+        <v>0</v>
+      </c>
+      <c r="P316" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q316" t="n">
+        <v>0</v>
+      </c>
+      <c r="R316" t="n">
+        <v>1</v>
+      </c>
+      <c r="S316" t="n">
+        <v>6</v>
+      </c>
+      <c r="T316" t="n">
+        <v>7</v>
+      </c>
+      <c r="U316" t="n">
+        <v>2</v>
+      </c>
+      <c r="V316" t="n">
+        <v>0</v>
+      </c>
+      <c r="W316" t="n">
+        <v>0</v>
+      </c>
+      <c r="X316" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y316" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z316" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA316" t="n">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>19:14</t>
+        </is>
+      </c>
+      <c r="I317" t="n">
+        <v>2</v>
+      </c>
+      <c r="J317" t="n">
+        <v>2</v>
+      </c>
+      <c r="K317" t="n">
+        <v>1</v>
+      </c>
+      <c r="L317" t="n">
+        <v>0</v>
+      </c>
+      <c r="M317" t="n">
+        <v>0</v>
+      </c>
+      <c r="N317" t="n">
+        <v>0</v>
+      </c>
+      <c r="O317" t="n">
+        <v>1</v>
+      </c>
+      <c r="P317" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q317" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R317" t="n">
+        <v>1</v>
+      </c>
+      <c r="S317" t="n">
+        <v>2</v>
+      </c>
+      <c r="T317" t="n">
+        <v>3</v>
+      </c>
+      <c r="U317" t="n">
+        <v>1</v>
+      </c>
+      <c r="V317" t="n">
+        <v>0</v>
+      </c>
+      <c r="W317" t="n">
+        <v>0</v>
+      </c>
+      <c r="X317" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y317" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z317" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA317" t="n">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>34:44</t>
+        </is>
+      </c>
+      <c r="I318" t="n">
+        <v>4</v>
+      </c>
+      <c r="J318" t="n">
+        <v>11</v>
+      </c>
+      <c r="K318" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="L318" t="n">
+        <v>2</v>
+      </c>
+      <c r="M318" t="n">
+        <v>6</v>
+      </c>
+      <c r="N318" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O318" t="n">
+        <v>3</v>
+      </c>
+      <c r="P318" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q318" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R318" t="n">
+        <v>1</v>
+      </c>
+      <c r="S318" t="n">
+        <v>3</v>
+      </c>
+      <c r="T318" t="n">
+        <v>4</v>
+      </c>
+      <c r="U318" t="n">
+        <v>1</v>
+      </c>
+      <c r="V318" t="n">
+        <v>2</v>
+      </c>
+      <c r="W318" t="n">
+        <v>0</v>
+      </c>
+      <c r="X318" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y318" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z318" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA318" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>33:01</t>
+        </is>
+      </c>
+      <c r="I319" t="n">
+        <v>3</v>
+      </c>
+      <c r="J319" t="n">
+        <v>14</v>
+      </c>
+      <c r="K319" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="L319" t="n">
+        <v>0</v>
+      </c>
+      <c r="M319" t="n">
+        <v>4</v>
+      </c>
+      <c r="N319" t="n">
+        <v>0</v>
+      </c>
+      <c r="O319" t="n">
+        <v>5</v>
+      </c>
+      <c r="P319" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q319" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="R319" t="n">
+        <v>1</v>
+      </c>
+      <c r="S319" t="n">
+        <v>2</v>
+      </c>
+      <c r="T319" t="n">
+        <v>3</v>
+      </c>
+      <c r="U319" t="n">
+        <v>1</v>
+      </c>
+      <c r="V319" t="n">
+        <v>4</v>
+      </c>
+      <c r="W319" t="n">
+        <v>0</v>
+      </c>
+      <c r="X319" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y319" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z319" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA319" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>15:52</t>
+        </is>
+      </c>
+      <c r="I320" t="n">
+        <v>1</v>
+      </c>
+      <c r="J320" t="n">
+        <v>5</v>
+      </c>
+      <c r="K320" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L320" t="n">
+        <v>1</v>
+      </c>
+      <c r="M320" t="n">
+        <v>2</v>
+      </c>
+      <c r="N320" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O320" t="n">
+        <v>0</v>
+      </c>
+      <c r="P320" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q320" t="n">
+        <v>0</v>
+      </c>
+      <c r="R320" t="n">
+        <v>3</v>
+      </c>
+      <c r="S320" t="n">
+        <v>0</v>
+      </c>
+      <c r="T320" t="n">
+        <v>3</v>
+      </c>
+      <c r="U320" t="n">
+        <v>2</v>
+      </c>
+      <c r="V320" t="n">
+        <v>1</v>
+      </c>
+      <c r="W320" t="n">
+        <v>0</v>
+      </c>
+      <c r="X320" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y320" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z320" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA320" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B321" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>29:31</t>
+        </is>
+      </c>
+      <c r="I321" t="n">
+        <v>6</v>
+      </c>
+      <c r="J321" t="n">
+        <v>13</v>
+      </c>
+      <c r="K321" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="L321" t="n">
+        <v>0</v>
+      </c>
+      <c r="M321" t="n">
+        <v>2</v>
+      </c>
+      <c r="N321" t="n">
+        <v>0</v>
+      </c>
+      <c r="O321" t="n">
+        <v>11</v>
+      </c>
+      <c r="P321" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q321" t="n">
+        <v>0.917</v>
+      </c>
+      <c r="R321" t="n">
+        <v>0</v>
+      </c>
+      <c r="S321" t="n">
+        <v>0</v>
+      </c>
+      <c r="T321" t="n">
+        <v>0</v>
+      </c>
+      <c r="U321" t="n">
+        <v>1</v>
+      </c>
+      <c r="V321" t="n">
+        <v>1</v>
+      </c>
+      <c r="W321" t="n">
+        <v>0</v>
+      </c>
+      <c r="X321" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y321" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z321" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA321" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B322" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="I322" t="n">
+        <v>3</v>
+      </c>
+      <c r="J322" t="n">
+        <v>5</v>
+      </c>
+      <c r="K322" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L322" t="n">
+        <v>0</v>
+      </c>
+      <c r="M322" t="n">
+        <v>0</v>
+      </c>
+      <c r="N322" t="n">
+        <v>0</v>
+      </c>
+      <c r="O322" t="n">
+        <v>2</v>
+      </c>
+      <c r="P322" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q322" t="n">
+        <v>1</v>
+      </c>
+      <c r="R322" t="n">
+        <v>3</v>
+      </c>
+      <c r="S322" t="n">
+        <v>5</v>
+      </c>
+      <c r="T322" t="n">
+        <v>8</v>
+      </c>
+      <c r="U322" t="n">
+        <v>0</v>
+      </c>
+      <c r="V322" t="n">
+        <v>0</v>
+      </c>
+      <c r="W322" t="n">
+        <v>0</v>
+      </c>
+      <c r="X322" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y322" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z322" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA322" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B323" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>0:08</t>
+        </is>
+      </c>
+      <c r="I323" t="n">
+        <v>0</v>
+      </c>
+      <c r="J323" t="n">
+        <v>0</v>
+      </c>
+      <c r="K323" t="n">
+        <v>0</v>
+      </c>
+      <c r="L323" t="n">
+        <v>0</v>
+      </c>
+      <c r="M323" t="n">
+        <v>0</v>
+      </c>
+      <c r="N323" t="n">
+        <v>0</v>
+      </c>
+      <c r="O323" t="n">
+        <v>0</v>
+      </c>
+      <c r="P323" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q323" t="n">
+        <v>0</v>
+      </c>
+      <c r="R323" t="n">
+        <v>0</v>
+      </c>
+      <c r="S323" t="n">
+        <v>0</v>
+      </c>
+      <c r="T323" t="n">
+        <v>0</v>
+      </c>
+      <c r="U323" t="n">
+        <v>0</v>
+      </c>
+      <c r="V323" t="n">
+        <v>0</v>
+      </c>
+      <c r="W323" t="n">
+        <v>0</v>
+      </c>
+      <c r="X323" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y323" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z323" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA323" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B324" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>6:53</t>
+        </is>
+      </c>
+      <c r="I324" t="n">
+        <v>1</v>
+      </c>
+      <c r="J324" t="n">
+        <v>3</v>
+      </c>
+      <c r="K324" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L324" t="n">
+        <v>1</v>
+      </c>
+      <c r="M324" t="n">
+        <v>3</v>
+      </c>
+      <c r="N324" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O324" t="n">
+        <v>0</v>
+      </c>
+      <c r="P324" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q324" t="n">
+        <v>0</v>
+      </c>
+      <c r="R324" t="n">
+        <v>0</v>
+      </c>
+      <c r="S324" t="n">
+        <v>1</v>
+      </c>
+      <c r="T324" t="n">
+        <v>1</v>
+      </c>
+      <c r="U324" t="n">
+        <v>3</v>
+      </c>
+      <c r="V324" t="n">
+        <v>0</v>
+      </c>
+      <c r="W324" t="n">
+        <v>0</v>
+      </c>
+      <c r="X324" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y324" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z324" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA324" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B325" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>4:38</t>
+        </is>
+      </c>
+      <c r="I325" t="n">
+        <v>0</v>
+      </c>
+      <c r="J325" t="n">
+        <v>0</v>
+      </c>
+      <c r="K325" t="n">
+        <v>0</v>
+      </c>
+      <c r="L325" t="n">
+        <v>0</v>
+      </c>
+      <c r="M325" t="n">
+        <v>0</v>
+      </c>
+      <c r="N325" t="n">
+        <v>0</v>
+      </c>
+      <c r="O325" t="n">
+        <v>2</v>
+      </c>
+      <c r="P325" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q325" t="n">
+        <v>1</v>
+      </c>
+      <c r="R325" t="n">
+        <v>0</v>
+      </c>
+      <c r="S325" t="n">
+        <v>0</v>
+      </c>
+      <c r="T325" t="n">
+        <v>0</v>
+      </c>
+      <c r="U325" t="n">
+        <v>0</v>
+      </c>
+      <c r="V325" t="n">
+        <v>0</v>
+      </c>
+      <c r="W325" t="n">
+        <v>0</v>
+      </c>
+      <c r="X325" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y325" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z325" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA325" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B326" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>4:38</t>
+        </is>
+      </c>
+      <c r="I326" t="n">
+        <v>1</v>
+      </c>
+      <c r="J326" t="n">
+        <v>1</v>
+      </c>
+      <c r="K326" t="n">
+        <v>1</v>
+      </c>
+      <c r="L326" t="n">
+        <v>0</v>
+      </c>
+      <c r="M326" t="n">
+        <v>0</v>
+      </c>
+      <c r="N326" t="n">
+        <v>0</v>
+      </c>
+      <c r="O326" t="n">
+        <v>0</v>
+      </c>
+      <c r="P326" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q326" t="n">
+        <v>0</v>
+      </c>
+      <c r="R326" t="n">
+        <v>0</v>
+      </c>
+      <c r="S326" t="n">
+        <v>0</v>
+      </c>
+      <c r="T326" t="n">
+        <v>0</v>
+      </c>
+      <c r="U326" t="n">
+        <v>1</v>
+      </c>
+      <c r="V326" t="n">
+        <v>0</v>
+      </c>
+      <c r="W326" t="n">
+        <v>0</v>
+      </c>
+      <c r="X326" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y326" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z326" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA326" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="B327" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>4:38</t>
+        </is>
+      </c>
+      <c r="I327" t="n">
+        <v>3</v>
+      </c>
+      <c r="J327" t="n">
+        <v>4</v>
+      </c>
+      <c r="K327" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L327" t="n">
+        <v>1</v>
+      </c>
+      <c r="M327" t="n">
+        <v>1</v>
+      </c>
+      <c r="N327" t="n">
+        <v>1</v>
+      </c>
+      <c r="O327" t="n">
+        <v>0</v>
+      </c>
+      <c r="P327" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q327" t="n">
+        <v>0</v>
+      </c>
+      <c r="R327" t="n">
+        <v>0</v>
+      </c>
+      <c r="S327" t="n">
+        <v>1</v>
+      </c>
+      <c r="T327" t="n">
+        <v>1</v>
+      </c>
+      <c r="U327" t="n">
+        <v>2</v>
+      </c>
+      <c r="V327" t="n">
+        <v>2</v>
+      </c>
+      <c r="W327" t="n">
+        <v>0</v>
+      </c>
+      <c r="X327" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y327" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z327" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA327" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B328" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>4:38</t>
+        </is>
+      </c>
+      <c r="I328" t="n">
+        <v>2</v>
+      </c>
+      <c r="J328" t="n">
+        <v>4</v>
+      </c>
+      <c r="K328" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L328" t="n">
+        <v>1</v>
+      </c>
+      <c r="M328" t="n">
+        <v>2</v>
+      </c>
+      <c r="N328" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O328" t="n">
+        <v>0</v>
+      </c>
+      <c r="P328" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q328" t="n">
+        <v>0</v>
+      </c>
+      <c r="R328" t="n">
+        <v>1</v>
+      </c>
+      <c r="S328" t="n">
+        <v>1</v>
+      </c>
+      <c r="T328" t="n">
+        <v>2</v>
+      </c>
+      <c r="U328" t="n">
+        <v>1</v>
+      </c>
+      <c r="V328" t="n">
+        <v>0</v>
+      </c>
+      <c r="W328" t="n">
+        <v>0</v>
+      </c>
+      <c r="X328" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y328" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z328" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA328" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B329" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="H329" t="inlineStr"/>
+      <c r="I329" t="n">
+        <v>0</v>
+      </c>
+      <c r="J329" t="n">
+        <v>0</v>
+      </c>
+      <c r="K329" t="n">
+        <v>0</v>
+      </c>
+      <c r="L329" t="n">
+        <v>0</v>
+      </c>
+      <c r="M329" t="n">
+        <v>0</v>
+      </c>
+      <c r="N329" t="n">
+        <v>0</v>
+      </c>
+      <c r="O329" t="n">
+        <v>0</v>
+      </c>
+      <c r="P329" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q329" t="n">
+        <v>0</v>
+      </c>
+      <c r="R329" t="n">
+        <v>0</v>
+      </c>
+      <c r="S329" t="n">
+        <v>0</v>
+      </c>
+      <c r="T329" t="n">
+        <v>0</v>
+      </c>
+      <c r="U329" t="n">
+        <v>0</v>
+      </c>
+      <c r="V329" t="n">
+        <v>0</v>
+      </c>
+      <c r="W329" t="n">
+        <v>0</v>
+      </c>
+      <c r="X329" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y329" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z329" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA329" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add GSW vs MIN GM5 stats & update spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_player_playoffs_stats.xlsx
+++ b/data/gsw_box_score_player_playoffs_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA329"/>
+  <dimension ref="A1:AA359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31393,6 +31393,2816 @@
         <v>0</v>
       </c>
     </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="B330" t="n">
+        <v>202710</v>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Jimmy Butler III</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>41:54</t>
+        </is>
+      </c>
+      <c r="I330" t="n">
+        <v>4</v>
+      </c>
+      <c r="J330" t="n">
+        <v>11</v>
+      </c>
+      <c r="K330" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="L330" t="n">
+        <v>0</v>
+      </c>
+      <c r="M330" t="n">
+        <v>3</v>
+      </c>
+      <c r="N330" t="n">
+        <v>0</v>
+      </c>
+      <c r="O330" t="n">
+        <v>9</v>
+      </c>
+      <c r="P330" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q330" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="R330" t="n">
+        <v>3</v>
+      </c>
+      <c r="S330" t="n">
+        <v>3</v>
+      </c>
+      <c r="T330" t="n">
+        <v>6</v>
+      </c>
+      <c r="U330" t="n">
+        <v>6</v>
+      </c>
+      <c r="V330" t="n">
+        <v>3</v>
+      </c>
+      <c r="W330" t="n">
+        <v>0</v>
+      </c>
+      <c r="X330" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y330" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z330" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA330" t="n">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="B331" t="n">
+        <v>203110</v>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>Draymond Green</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>35:46</t>
+        </is>
+      </c>
+      <c r="I331" t="n">
+        <v>4</v>
+      </c>
+      <c r="J331" t="n">
+        <v>11</v>
+      </c>
+      <c r="K331" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="L331" t="n">
+        <v>1</v>
+      </c>
+      <c r="M331" t="n">
+        <v>6</v>
+      </c>
+      <c r="N331" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="O331" t="n">
+        <v>1</v>
+      </c>
+      <c r="P331" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q331" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R331" t="n">
+        <v>2</v>
+      </c>
+      <c r="S331" t="n">
+        <v>4</v>
+      </c>
+      <c r="T331" t="n">
+        <v>6</v>
+      </c>
+      <c r="U331" t="n">
+        <v>6</v>
+      </c>
+      <c r="V331" t="n">
+        <v>1</v>
+      </c>
+      <c r="W331" t="n">
+        <v>0</v>
+      </c>
+      <c r="X331" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y331" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z331" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA331" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="B332" t="n">
+        <v>1631218</v>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Trayce Jackson-Davis</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>6:41</t>
+        </is>
+      </c>
+      <c r="I332" t="n">
+        <v>1</v>
+      </c>
+      <c r="J332" t="n">
+        <v>1</v>
+      </c>
+      <c r="K332" t="n">
+        <v>1</v>
+      </c>
+      <c r="L332" t="n">
+        <v>0</v>
+      </c>
+      <c r="M332" t="n">
+        <v>0</v>
+      </c>
+      <c r="N332" t="n">
+        <v>0</v>
+      </c>
+      <c r="O332" t="n">
+        <v>0</v>
+      </c>
+      <c r="P332" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q332" t="n">
+        <v>0</v>
+      </c>
+      <c r="R332" t="n">
+        <v>2</v>
+      </c>
+      <c r="S332" t="n">
+        <v>0</v>
+      </c>
+      <c r="T332" t="n">
+        <v>2</v>
+      </c>
+      <c r="U332" t="n">
+        <v>0</v>
+      </c>
+      <c r="V332" t="n">
+        <v>1</v>
+      </c>
+      <c r="W332" t="n">
+        <v>0</v>
+      </c>
+      <c r="X332" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y332" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z332" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA332" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="B333" t="n">
+        <v>1627741</v>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Buddy Hield</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>29:37</t>
+        </is>
+      </c>
+      <c r="I333" t="n">
+        <v>2</v>
+      </c>
+      <c r="J333" t="n">
+        <v>9</v>
+      </c>
+      <c r="K333" t="n">
+        <v>0.222</v>
+      </c>
+      <c r="L333" t="n">
+        <v>0</v>
+      </c>
+      <c r="M333" t="n">
+        <v>4</v>
+      </c>
+      <c r="N333" t="n">
+        <v>0</v>
+      </c>
+      <c r="O333" t="n">
+        <v>4</v>
+      </c>
+      <c r="P333" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q333" t="n">
+        <v>1</v>
+      </c>
+      <c r="R333" t="n">
+        <v>2</v>
+      </c>
+      <c r="S333" t="n">
+        <v>2</v>
+      </c>
+      <c r="T333" t="n">
+        <v>4</v>
+      </c>
+      <c r="U333" t="n">
+        <v>1</v>
+      </c>
+      <c r="V333" t="n">
+        <v>2</v>
+      </c>
+      <c r="W333" t="n">
+        <v>0</v>
+      </c>
+      <c r="X333" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y333" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z333" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA333" t="n">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>332</v>
+      </c>
+      <c r="B334" t="n">
+        <v>1641764</v>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Brandin Podziemski</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H334" t="inlineStr">
+        <is>
+          <t>38:44</t>
+        </is>
+      </c>
+      <c r="I334" t="n">
+        <v>11</v>
+      </c>
+      <c r="J334" t="n">
+        <v>19</v>
+      </c>
+      <c r="K334" t="n">
+        <v>0.579</v>
+      </c>
+      <c r="L334" t="n">
+        <v>4</v>
+      </c>
+      <c r="M334" t="n">
+        <v>6</v>
+      </c>
+      <c r="N334" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O334" t="n">
+        <v>2</v>
+      </c>
+      <c r="P334" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q334" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="R334" t="n">
+        <v>2</v>
+      </c>
+      <c r="S334" t="n">
+        <v>4</v>
+      </c>
+      <c r="T334" t="n">
+        <v>6</v>
+      </c>
+      <c r="U334" t="n">
+        <v>4</v>
+      </c>
+      <c r="V334" t="n">
+        <v>2</v>
+      </c>
+      <c r="W334" t="n">
+        <v>0</v>
+      </c>
+      <c r="X334" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y334" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z334" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA334" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="B335" t="n">
+        <v>1630228</v>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Jonathan Kuminga</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>32:14</t>
+        </is>
+      </c>
+      <c r="I335" t="n">
+        <v>11</v>
+      </c>
+      <c r="J335" t="n">
+        <v>23</v>
+      </c>
+      <c r="K335" t="n">
+        <v>0.478</v>
+      </c>
+      <c r="L335" t="n">
+        <v>3</v>
+      </c>
+      <c r="M335" t="n">
+        <v>9</v>
+      </c>
+      <c r="N335" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O335" t="n">
+        <v>1</v>
+      </c>
+      <c r="P335" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q335" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="R335" t="n">
+        <v>1</v>
+      </c>
+      <c r="S335" t="n">
+        <v>2</v>
+      </c>
+      <c r="T335" t="n">
+        <v>3</v>
+      </c>
+      <c r="U335" t="n">
+        <v>0</v>
+      </c>
+      <c r="V335" t="n">
+        <v>2</v>
+      </c>
+      <c r="W335" t="n">
+        <v>0</v>
+      </c>
+      <c r="X335" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y335" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z335" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA335" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B336" t="n">
+        <v>1627780</v>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Gary Payton II</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>5:42</t>
+        </is>
+      </c>
+      <c r="I336" t="n">
+        <v>0</v>
+      </c>
+      <c r="J336" t="n">
+        <v>0</v>
+      </c>
+      <c r="K336" t="n">
+        <v>0</v>
+      </c>
+      <c r="L336" t="n">
+        <v>0</v>
+      </c>
+      <c r="M336" t="n">
+        <v>0</v>
+      </c>
+      <c r="N336" t="n">
+        <v>0</v>
+      </c>
+      <c r="O336" t="n">
+        <v>0</v>
+      </c>
+      <c r="P336" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q336" t="n">
+        <v>0</v>
+      </c>
+      <c r="R336" t="n">
+        <v>0</v>
+      </c>
+      <c r="S336" t="n">
+        <v>0</v>
+      </c>
+      <c r="T336" t="n">
+        <v>0</v>
+      </c>
+      <c r="U336" t="n">
+        <v>0</v>
+      </c>
+      <c r="V336" t="n">
+        <v>1</v>
+      </c>
+      <c r="W336" t="n">
+        <v>0</v>
+      </c>
+      <c r="X336" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y336" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z336" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA336" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>335</v>
+      </c>
+      <c r="B337" t="n">
+        <v>1630611</v>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Gui Santos</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>15:43</t>
+        </is>
+      </c>
+      <c r="I337" t="n">
+        <v>1</v>
+      </c>
+      <c r="J337" t="n">
+        <v>4</v>
+      </c>
+      <c r="K337" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L337" t="n">
+        <v>0</v>
+      </c>
+      <c r="M337" t="n">
+        <v>3</v>
+      </c>
+      <c r="N337" t="n">
+        <v>0</v>
+      </c>
+      <c r="O337" t="n">
+        <v>0</v>
+      </c>
+      <c r="P337" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q337" t="n">
+        <v>0</v>
+      </c>
+      <c r="R337" t="n">
+        <v>3</v>
+      </c>
+      <c r="S337" t="n">
+        <v>2</v>
+      </c>
+      <c r="T337" t="n">
+        <v>5</v>
+      </c>
+      <c r="U337" t="n">
+        <v>0</v>
+      </c>
+      <c r="V337" t="n">
+        <v>0</v>
+      </c>
+      <c r="W337" t="n">
+        <v>1</v>
+      </c>
+      <c r="X337" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y337" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z337" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA337" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="B338" t="n">
+        <v>1626172</v>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Kevon Looney</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>5:59</t>
+        </is>
+      </c>
+      <c r="I338" t="n">
+        <v>0</v>
+      </c>
+      <c r="J338" t="n">
+        <v>0</v>
+      </c>
+      <c r="K338" t="n">
+        <v>0</v>
+      </c>
+      <c r="L338" t="n">
+        <v>0</v>
+      </c>
+      <c r="M338" t="n">
+        <v>0</v>
+      </c>
+      <c r="N338" t="n">
+        <v>0</v>
+      </c>
+      <c r="O338" t="n">
+        <v>0</v>
+      </c>
+      <c r="P338" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q338" t="n">
+        <v>0</v>
+      </c>
+      <c r="R338" t="n">
+        <v>1</v>
+      </c>
+      <c r="S338" t="n">
+        <v>2</v>
+      </c>
+      <c r="T338" t="n">
+        <v>3</v>
+      </c>
+      <c r="U338" t="n">
+        <v>1</v>
+      </c>
+      <c r="V338" t="n">
+        <v>0</v>
+      </c>
+      <c r="W338" t="n">
+        <v>0</v>
+      </c>
+      <c r="X338" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y338" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z338" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA338" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>337</v>
+      </c>
+      <c r="B339" t="n">
+        <v>1642366</v>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Quinten Post</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>9:56</t>
+        </is>
+      </c>
+      <c r="I339" t="n">
+        <v>1</v>
+      </c>
+      <c r="J339" t="n">
+        <v>4</v>
+      </c>
+      <c r="K339" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L339" t="n">
+        <v>1</v>
+      </c>
+      <c r="M339" t="n">
+        <v>4</v>
+      </c>
+      <c r="N339" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O339" t="n">
+        <v>0</v>
+      </c>
+      <c r="P339" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q339" t="n">
+        <v>0</v>
+      </c>
+      <c r="R339" t="n">
+        <v>0</v>
+      </c>
+      <c r="S339" t="n">
+        <v>3</v>
+      </c>
+      <c r="T339" t="n">
+        <v>3</v>
+      </c>
+      <c r="U339" t="n">
+        <v>0</v>
+      </c>
+      <c r="V339" t="n">
+        <v>0</v>
+      </c>
+      <c r="W339" t="n">
+        <v>0</v>
+      </c>
+      <c r="X339" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y339" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z339" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA339" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="B340" t="n">
+        <v>1630311</v>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Pat Spencer</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>5:44</t>
+        </is>
+      </c>
+      <c r="I340" t="n">
+        <v>1</v>
+      </c>
+      <c r="J340" t="n">
+        <v>2</v>
+      </c>
+      <c r="K340" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L340" t="n">
+        <v>0</v>
+      </c>
+      <c r="M340" t="n">
+        <v>1</v>
+      </c>
+      <c r="N340" t="n">
+        <v>0</v>
+      </c>
+      <c r="O340" t="n">
+        <v>0</v>
+      </c>
+      <c r="P340" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q340" t="n">
+        <v>0</v>
+      </c>
+      <c r="R340" t="n">
+        <v>1</v>
+      </c>
+      <c r="S340" t="n">
+        <v>0</v>
+      </c>
+      <c r="T340" t="n">
+        <v>1</v>
+      </c>
+      <c r="U340" t="n">
+        <v>1</v>
+      </c>
+      <c r="V340" t="n">
+        <v>0</v>
+      </c>
+      <c r="W340" t="n">
+        <v>0</v>
+      </c>
+      <c r="X340" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y340" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z340" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA340" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B341" t="n">
+        <v>1630541</v>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Moses Moody</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="I341" t="n">
+        <v>3</v>
+      </c>
+      <c r="J341" t="n">
+        <v>6</v>
+      </c>
+      <c r="K341" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L341" t="n">
+        <v>2</v>
+      </c>
+      <c r="M341" t="n">
+        <v>3</v>
+      </c>
+      <c r="N341" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O341" t="n">
+        <v>4</v>
+      </c>
+      <c r="P341" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q341" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R341" t="n">
+        <v>1</v>
+      </c>
+      <c r="S341" t="n">
+        <v>0</v>
+      </c>
+      <c r="T341" t="n">
+        <v>1</v>
+      </c>
+      <c r="U341" t="n">
+        <v>2</v>
+      </c>
+      <c r="V341" t="n">
+        <v>2</v>
+      </c>
+      <c r="W341" t="n">
+        <v>0</v>
+      </c>
+      <c r="X341" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y341" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z341" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA341" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B342" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Stephen Curry</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr"/>
+      <c r="I342" t="n">
+        <v>0</v>
+      </c>
+      <c r="J342" t="n">
+        <v>0</v>
+      </c>
+      <c r="K342" t="n">
+        <v>0</v>
+      </c>
+      <c r="L342" t="n">
+        <v>0</v>
+      </c>
+      <c r="M342" t="n">
+        <v>0</v>
+      </c>
+      <c r="N342" t="n">
+        <v>0</v>
+      </c>
+      <c r="O342" t="n">
+        <v>0</v>
+      </c>
+      <c r="P342" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q342" t="n">
+        <v>0</v>
+      </c>
+      <c r="R342" t="n">
+        <v>0</v>
+      </c>
+      <c r="S342" t="n">
+        <v>0</v>
+      </c>
+      <c r="T342" t="n">
+        <v>0</v>
+      </c>
+      <c r="U342" t="n">
+        <v>0</v>
+      </c>
+      <c r="V342" t="n">
+        <v>0</v>
+      </c>
+      <c r="W342" t="n">
+        <v>0</v>
+      </c>
+      <c r="X342" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y342" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z342" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA342" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B343" t="n">
+        <v>1630296</v>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Braxton Key</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr"/>
+      <c r="I343" t="n">
+        <v>0</v>
+      </c>
+      <c r="J343" t="n">
+        <v>0</v>
+      </c>
+      <c r="K343" t="n">
+        <v>0</v>
+      </c>
+      <c r="L343" t="n">
+        <v>0</v>
+      </c>
+      <c r="M343" t="n">
+        <v>0</v>
+      </c>
+      <c r="N343" t="n">
+        <v>0</v>
+      </c>
+      <c r="O343" t="n">
+        <v>0</v>
+      </c>
+      <c r="P343" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q343" t="n">
+        <v>0</v>
+      </c>
+      <c r="R343" t="n">
+        <v>0</v>
+      </c>
+      <c r="S343" t="n">
+        <v>0</v>
+      </c>
+      <c r="T343" t="n">
+        <v>0</v>
+      </c>
+      <c r="U343" t="n">
+        <v>0</v>
+      </c>
+      <c r="V343" t="n">
+        <v>0</v>
+      </c>
+      <c r="W343" t="n">
+        <v>0</v>
+      </c>
+      <c r="X343" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y343" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z343" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA343" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B344" t="n">
+        <v>1628995</v>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Kevin Knox II</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr"/>
+      <c r="I344" t="n">
+        <v>0</v>
+      </c>
+      <c r="J344" t="n">
+        <v>0</v>
+      </c>
+      <c r="K344" t="n">
+        <v>0</v>
+      </c>
+      <c r="L344" t="n">
+        <v>0</v>
+      </c>
+      <c r="M344" t="n">
+        <v>0</v>
+      </c>
+      <c r="N344" t="n">
+        <v>0</v>
+      </c>
+      <c r="O344" t="n">
+        <v>0</v>
+      </c>
+      <c r="P344" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q344" t="n">
+        <v>0</v>
+      </c>
+      <c r="R344" t="n">
+        <v>0</v>
+      </c>
+      <c r="S344" t="n">
+        <v>0</v>
+      </c>
+      <c r="T344" t="n">
+        <v>0</v>
+      </c>
+      <c r="U344" t="n">
+        <v>0</v>
+      </c>
+      <c r="V344" t="n">
+        <v>0</v>
+      </c>
+      <c r="W344" t="n">
+        <v>0</v>
+      </c>
+      <c r="X344" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y344" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z344" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA344" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="B345" t="n">
+        <v>1630183</v>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Jaden McDaniels</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>41:05</t>
+        </is>
+      </c>
+      <c r="I345" t="n">
+        <v>6</v>
+      </c>
+      <c r="J345" t="n">
+        <v>14</v>
+      </c>
+      <c r="K345" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="L345" t="n">
+        <v>0</v>
+      </c>
+      <c r="M345" t="n">
+        <v>3</v>
+      </c>
+      <c r="N345" t="n">
+        <v>0</v>
+      </c>
+      <c r="O345" t="n">
+        <v>2</v>
+      </c>
+      <c r="P345" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q345" t="n">
+        <v>1</v>
+      </c>
+      <c r="R345" t="n">
+        <v>1</v>
+      </c>
+      <c r="S345" t="n">
+        <v>3</v>
+      </c>
+      <c r="T345" t="n">
+        <v>4</v>
+      </c>
+      <c r="U345" t="n">
+        <v>2</v>
+      </c>
+      <c r="V345" t="n">
+        <v>4</v>
+      </c>
+      <c r="W345" t="n">
+        <v>0</v>
+      </c>
+      <c r="X345" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y345" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z345" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA345" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B346" t="n">
+        <v>203944</v>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Julius Randle</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>42:30</t>
+        </is>
+      </c>
+      <c r="I346" t="n">
+        <v>13</v>
+      </c>
+      <c r="J346" t="n">
+        <v>18</v>
+      </c>
+      <c r="K346" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="L346" t="n">
+        <v>2</v>
+      </c>
+      <c r="M346" t="n">
+        <v>6</v>
+      </c>
+      <c r="N346" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O346" t="n">
+        <v>1</v>
+      </c>
+      <c r="P346" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q346" t="n">
+        <v>1</v>
+      </c>
+      <c r="R346" t="n">
+        <v>2</v>
+      </c>
+      <c r="S346" t="n">
+        <v>6</v>
+      </c>
+      <c r="T346" t="n">
+        <v>8</v>
+      </c>
+      <c r="U346" t="n">
+        <v>5</v>
+      </c>
+      <c r="V346" t="n">
+        <v>0</v>
+      </c>
+      <c r="W346" t="n">
+        <v>0</v>
+      </c>
+      <c r="X346" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y346" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z346" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA346" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="B347" t="n">
+        <v>203497</v>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Rudy Gobert</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>27:31</t>
+        </is>
+      </c>
+      <c r="I347" t="n">
+        <v>8</v>
+      </c>
+      <c r="J347" t="n">
+        <v>9</v>
+      </c>
+      <c r="K347" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="L347" t="n">
+        <v>0</v>
+      </c>
+      <c r="M347" t="n">
+        <v>0</v>
+      </c>
+      <c r="N347" t="n">
+        <v>0</v>
+      </c>
+      <c r="O347" t="n">
+        <v>1</v>
+      </c>
+      <c r="P347" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q347" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R347" t="n">
+        <v>0</v>
+      </c>
+      <c r="S347" t="n">
+        <v>8</v>
+      </c>
+      <c r="T347" t="n">
+        <v>8</v>
+      </c>
+      <c r="U347" t="n">
+        <v>0</v>
+      </c>
+      <c r="V347" t="n">
+        <v>0</v>
+      </c>
+      <c r="W347" t="n">
+        <v>1</v>
+      </c>
+      <c r="X347" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y347" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z347" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA347" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="B348" t="n">
+        <v>1630162</v>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Anthony Edwards</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H348" t="inlineStr">
+        <is>
+          <t>41:09</t>
+        </is>
+      </c>
+      <c r="I348" t="n">
+        <v>8</v>
+      </c>
+      <c r="J348" t="n">
+        <v>15</v>
+      </c>
+      <c r="K348" t="n">
+        <v>0.533</v>
+      </c>
+      <c r="L348" t="n">
+        <v>5</v>
+      </c>
+      <c r="M348" t="n">
+        <v>9</v>
+      </c>
+      <c r="N348" t="n">
+        <v>0.556</v>
+      </c>
+      <c r="O348" t="n">
+        <v>1</v>
+      </c>
+      <c r="P348" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q348" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R348" t="n">
+        <v>1</v>
+      </c>
+      <c r="S348" t="n">
+        <v>6</v>
+      </c>
+      <c r="T348" t="n">
+        <v>7</v>
+      </c>
+      <c r="U348" t="n">
+        <v>12</v>
+      </c>
+      <c r="V348" t="n">
+        <v>1</v>
+      </c>
+      <c r="W348" t="n">
+        <v>3</v>
+      </c>
+      <c r="X348" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y348" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z348" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA348" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>347</v>
+      </c>
+      <c r="B349" t="n">
+        <v>201144</v>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Mike Conley</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H349" t="inlineStr">
+        <is>
+          <t>26:30</t>
+        </is>
+      </c>
+      <c r="I349" t="n">
+        <v>5</v>
+      </c>
+      <c r="J349" t="n">
+        <v>7</v>
+      </c>
+      <c r="K349" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="L349" t="n">
+        <v>4</v>
+      </c>
+      <c r="M349" t="n">
+        <v>6</v>
+      </c>
+      <c r="N349" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O349" t="n">
+        <v>2</v>
+      </c>
+      <c r="P349" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q349" t="n">
+        <v>1</v>
+      </c>
+      <c r="R349" t="n">
+        <v>1</v>
+      </c>
+      <c r="S349" t="n">
+        <v>5</v>
+      </c>
+      <c r="T349" t="n">
+        <v>6</v>
+      </c>
+      <c r="U349" t="n">
+        <v>8</v>
+      </c>
+      <c r="V349" t="n">
+        <v>1</v>
+      </c>
+      <c r="W349" t="n">
+        <v>0</v>
+      </c>
+      <c r="X349" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y349" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z349" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA349" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="B350" t="n">
+        <v>1629675</v>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Naz Reid</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="I350" t="n">
+        <v>3</v>
+      </c>
+      <c r="J350" t="n">
+        <v>5</v>
+      </c>
+      <c r="K350" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L350" t="n">
+        <v>0</v>
+      </c>
+      <c r="M350" t="n">
+        <v>2</v>
+      </c>
+      <c r="N350" t="n">
+        <v>0</v>
+      </c>
+      <c r="O350" t="n">
+        <v>2</v>
+      </c>
+      <c r="P350" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q350" t="n">
+        <v>1</v>
+      </c>
+      <c r="R350" t="n">
+        <v>1</v>
+      </c>
+      <c r="S350" t="n">
+        <v>3</v>
+      </c>
+      <c r="T350" t="n">
+        <v>4</v>
+      </c>
+      <c r="U350" t="n">
+        <v>1</v>
+      </c>
+      <c r="V350" t="n">
+        <v>1</v>
+      </c>
+      <c r="W350" t="n">
+        <v>0</v>
+      </c>
+      <c r="X350" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y350" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z350" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA350" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="B351" t="n">
+        <v>1628978</v>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Donte DiVincenzo</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>26:27</t>
+        </is>
+      </c>
+      <c r="I351" t="n">
+        <v>5</v>
+      </c>
+      <c r="J351" t="n">
+        <v>7</v>
+      </c>
+      <c r="K351" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="L351" t="n">
+        <v>2</v>
+      </c>
+      <c r="M351" t="n">
+        <v>4</v>
+      </c>
+      <c r="N351" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O351" t="n">
+        <v>1</v>
+      </c>
+      <c r="P351" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q351" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R351" t="n">
+        <v>0</v>
+      </c>
+      <c r="S351" t="n">
+        <v>2</v>
+      </c>
+      <c r="T351" t="n">
+        <v>2</v>
+      </c>
+      <c r="U351" t="n">
+        <v>6</v>
+      </c>
+      <c r="V351" t="n">
+        <v>4</v>
+      </c>
+      <c r="W351" t="n">
+        <v>0</v>
+      </c>
+      <c r="X351" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y351" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z351" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA351" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B352" t="n">
+        <v>1629638</v>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="I352" t="n">
+        <v>1</v>
+      </c>
+      <c r="J352" t="n">
+        <v>3</v>
+      </c>
+      <c r="K352" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="L352" t="n">
+        <v>0</v>
+      </c>
+      <c r="M352" t="n">
+        <v>1</v>
+      </c>
+      <c r="N352" t="n">
+        <v>0</v>
+      </c>
+      <c r="O352" t="n">
+        <v>0</v>
+      </c>
+      <c r="P352" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q352" t="n">
+        <v>0</v>
+      </c>
+      <c r="R352" t="n">
+        <v>0</v>
+      </c>
+      <c r="S352" t="n">
+        <v>0</v>
+      </c>
+      <c r="T352" t="n">
+        <v>0</v>
+      </c>
+      <c r="U352" t="n">
+        <v>2</v>
+      </c>
+      <c r="V352" t="n">
+        <v>0</v>
+      </c>
+      <c r="W352" t="n">
+        <v>0</v>
+      </c>
+      <c r="X352" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y352" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z352" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA352" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B353" t="n">
+        <v>1641740</v>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>Jaylen Clark</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H353" t="inlineStr"/>
+      <c r="I353" t="n">
+        <v>0</v>
+      </c>
+      <c r="J353" t="n">
+        <v>0</v>
+      </c>
+      <c r="K353" t="n">
+        <v>0</v>
+      </c>
+      <c r="L353" t="n">
+        <v>0</v>
+      </c>
+      <c r="M353" t="n">
+        <v>0</v>
+      </c>
+      <c r="N353" t="n">
+        <v>0</v>
+      </c>
+      <c r="O353" t="n">
+        <v>0</v>
+      </c>
+      <c r="P353" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q353" t="n">
+        <v>0</v>
+      </c>
+      <c r="R353" t="n">
+        <v>0</v>
+      </c>
+      <c r="S353" t="n">
+        <v>0</v>
+      </c>
+      <c r="T353" t="n">
+        <v>0</v>
+      </c>
+      <c r="U353" t="n">
+        <v>0</v>
+      </c>
+      <c r="V353" t="n">
+        <v>0</v>
+      </c>
+      <c r="W353" t="n">
+        <v>0</v>
+      </c>
+      <c r="X353" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y353" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z353" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA353" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B354" t="n">
+        <v>1642265</v>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Rob Dillingham</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H354" t="inlineStr"/>
+      <c r="I354" t="n">
+        <v>0</v>
+      </c>
+      <c r="J354" t="n">
+        <v>0</v>
+      </c>
+      <c r="K354" t="n">
+        <v>0</v>
+      </c>
+      <c r="L354" t="n">
+        <v>0</v>
+      </c>
+      <c r="M354" t="n">
+        <v>0</v>
+      </c>
+      <c r="N354" t="n">
+        <v>0</v>
+      </c>
+      <c r="O354" t="n">
+        <v>0</v>
+      </c>
+      <c r="P354" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q354" t="n">
+        <v>0</v>
+      </c>
+      <c r="R354" t="n">
+        <v>0</v>
+      </c>
+      <c r="S354" t="n">
+        <v>0</v>
+      </c>
+      <c r="T354" t="n">
+        <v>0</v>
+      </c>
+      <c r="U354" t="n">
+        <v>0</v>
+      </c>
+      <c r="V354" t="n">
+        <v>0</v>
+      </c>
+      <c r="W354" t="n">
+        <v>0</v>
+      </c>
+      <c r="X354" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y354" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z354" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA354" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="B355" t="n">
+        <v>1630568</v>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>Luka Garza</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H355" t="inlineStr"/>
+      <c r="I355" t="n">
+        <v>0</v>
+      </c>
+      <c r="J355" t="n">
+        <v>0</v>
+      </c>
+      <c r="K355" t="n">
+        <v>0</v>
+      </c>
+      <c r="L355" t="n">
+        <v>0</v>
+      </c>
+      <c r="M355" t="n">
+        <v>0</v>
+      </c>
+      <c r="N355" t="n">
+        <v>0</v>
+      </c>
+      <c r="O355" t="n">
+        <v>0</v>
+      </c>
+      <c r="P355" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q355" t="n">
+        <v>0</v>
+      </c>
+      <c r="R355" t="n">
+        <v>0</v>
+      </c>
+      <c r="S355" t="n">
+        <v>0</v>
+      </c>
+      <c r="T355" t="n">
+        <v>0</v>
+      </c>
+      <c r="U355" t="n">
+        <v>0</v>
+      </c>
+      <c r="V355" t="n">
+        <v>0</v>
+      </c>
+      <c r="W355" t="n">
+        <v>0</v>
+      </c>
+      <c r="X355" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y355" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z355" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA355" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B356" t="n">
+        <v>204060</v>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>Joe Ingles</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr"/>
+      <c r="I356" t="n">
+        <v>0</v>
+      </c>
+      <c r="J356" t="n">
+        <v>0</v>
+      </c>
+      <c r="K356" t="n">
+        <v>0</v>
+      </c>
+      <c r="L356" t="n">
+        <v>0</v>
+      </c>
+      <c r="M356" t="n">
+        <v>0</v>
+      </c>
+      <c r="N356" t="n">
+        <v>0</v>
+      </c>
+      <c r="O356" t="n">
+        <v>0</v>
+      </c>
+      <c r="P356" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q356" t="n">
+        <v>0</v>
+      </c>
+      <c r="R356" t="n">
+        <v>0</v>
+      </c>
+      <c r="S356" t="n">
+        <v>0</v>
+      </c>
+      <c r="T356" t="n">
+        <v>0</v>
+      </c>
+      <c r="U356" t="n">
+        <v>0</v>
+      </c>
+      <c r="V356" t="n">
+        <v>0</v>
+      </c>
+      <c r="W356" t="n">
+        <v>0</v>
+      </c>
+      <c r="X356" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y356" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z356" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA356" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="B357" t="n">
+        <v>1631159</v>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>Leonard Miller</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H357" t="inlineStr"/>
+      <c r="I357" t="n">
+        <v>0</v>
+      </c>
+      <c r="J357" t="n">
+        <v>0</v>
+      </c>
+      <c r="K357" t="n">
+        <v>0</v>
+      </c>
+      <c r="L357" t="n">
+        <v>0</v>
+      </c>
+      <c r="M357" t="n">
+        <v>0</v>
+      </c>
+      <c r="N357" t="n">
+        <v>0</v>
+      </c>
+      <c r="O357" t="n">
+        <v>0</v>
+      </c>
+      <c r="P357" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q357" t="n">
+        <v>0</v>
+      </c>
+      <c r="R357" t="n">
+        <v>0</v>
+      </c>
+      <c r="S357" t="n">
+        <v>0</v>
+      </c>
+      <c r="T357" t="n">
+        <v>0</v>
+      </c>
+      <c r="U357" t="n">
+        <v>0</v>
+      </c>
+      <c r="V357" t="n">
+        <v>0</v>
+      </c>
+      <c r="W357" t="n">
+        <v>0</v>
+      </c>
+      <c r="X357" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y357" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z357" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA357" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="B358" t="n">
+        <v>1631169</v>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>Josh Minott</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H358" t="inlineStr"/>
+      <c r="I358" t="n">
+        <v>0</v>
+      </c>
+      <c r="J358" t="n">
+        <v>0</v>
+      </c>
+      <c r="K358" t="n">
+        <v>0</v>
+      </c>
+      <c r="L358" t="n">
+        <v>0</v>
+      </c>
+      <c r="M358" t="n">
+        <v>0</v>
+      </c>
+      <c r="N358" t="n">
+        <v>0</v>
+      </c>
+      <c r="O358" t="n">
+        <v>0</v>
+      </c>
+      <c r="P358" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q358" t="n">
+        <v>0</v>
+      </c>
+      <c r="R358" t="n">
+        <v>0</v>
+      </c>
+      <c r="S358" t="n">
+        <v>0</v>
+      </c>
+      <c r="T358" t="n">
+        <v>0</v>
+      </c>
+      <c r="U358" t="n">
+        <v>0</v>
+      </c>
+      <c r="V358" t="n">
+        <v>0</v>
+      </c>
+      <c r="W358" t="n">
+        <v>0</v>
+      </c>
+      <c r="X358" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y358" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z358" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA358" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B359" t="n">
+        <v>1630545</v>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>Terrence Shannon Jr.</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="H359" t="inlineStr"/>
+      <c r="I359" t="n">
+        <v>0</v>
+      </c>
+      <c r="J359" t="n">
+        <v>0</v>
+      </c>
+      <c r="K359" t="n">
+        <v>0</v>
+      </c>
+      <c r="L359" t="n">
+        <v>0</v>
+      </c>
+      <c r="M359" t="n">
+        <v>0</v>
+      </c>
+      <c r="N359" t="n">
+        <v>0</v>
+      </c>
+      <c r="O359" t="n">
+        <v>0</v>
+      </c>
+      <c r="P359" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q359" t="n">
+        <v>0</v>
+      </c>
+      <c r="R359" t="n">
+        <v>0</v>
+      </c>
+      <c r="S359" t="n">
+        <v>0</v>
+      </c>
+      <c r="T359" t="n">
+        <v>0</v>
+      </c>
+      <c r="U359" t="n">
+        <v>0</v>
+      </c>
+      <c r="V359" t="n">
+        <v>0</v>
+      </c>
+      <c r="W359" t="n">
+        <v>0</v>
+      </c>
+      <c r="X359" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y359" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z359" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA359" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>